<commit_message>
Updated FRA model - 2025-07-29 00:44
</commit_message>
<xml_diff>
--- a/VerveStacks_FRA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_FRA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FRA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F6547B-089F-4D6F-8A69-B4848DD83882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A503EE-1898-47B6-B5CF-C67C458B1EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -47,16 +48,40 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="87">
   <si>
     <t>bioenergy</t>
   </si>
@@ -250,7 +275,73 @@
     <t>-CO2Captured</t>
   </si>
   <si>
+    <t>Unnamed: 8</t>
+  </si>
+  <si>
+    <t>Unnamed: 9</t>
+  </si>
+  <si>
+    <t>Unnamed: 10</t>
+  </si>
+  <si>
+    <t>Unnamed: 11</t>
+  </si>
+  <si>
+    <t>Unnamed: 12</t>
+  </si>
+  <si>
+    <t>Unnamed: 13</t>
+  </si>
+  <si>
+    <t>Unnamed: 14</t>
+  </si>
+  <si>
+    <t>Unnamed: 15</t>
+  </si>
+  <si>
+    <t>Unnamed: 16</t>
+  </si>
+  <si>
+    <t>Unnamed: 17</t>
+  </si>
+  <si>
+    <t>Unnamed: 18</t>
+  </si>
+  <si>
+    <t>Unnamed: 19</t>
+  </si>
+  <si>
+    <t>Unnamed: 20</t>
+  </si>
+  <si>
+    <t>Unnamed: 21</t>
+  </si>
+  <si>
+    <t>Unnamed: 22</t>
+  </si>
+  <si>
+    <t>Unnamed: 23</t>
+  </si>
+  <si>
+    <t>Unnamed: 24</t>
+  </si>
+  <si>
+    <t>Unnamed: 25</t>
+  </si>
+  <si>
     <t>FRA</t>
+  </si>
+  <si>
+    <t>Electricity Trade Data (TWh)</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Export</t>
   </si>
 </sst>
 </file>
@@ -318,6 +409,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+  <rv s="1">
+    <v>13</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,14 +875,14 @@
       <c r="P4" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="4" cm="1">
+      <c r="Q4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q4">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>0.43129337356808434</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="4" cm="1">
+      <c r="S4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S4">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>9.4315434766683762E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.45">
@@ -748,17 +905,17 @@
       <c r="P5" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="4" cm="1">
+      <c r="Q5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q5">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>0.29350540681363757</v>
-      </c>
-      <c r="R5" s="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="4" t="e" vm="2">
         <f>IF(Q5&gt;0.7,Q5,0.7)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S5" s="4" cm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S5">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>5.1995525945360881E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.45">
@@ -868,9 +1025,9 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="3" t="e" vm="2">
         <f>-Q4*$Q$1*8.76</f>
-        <v>-4.1559429477020604</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z8" s="3"/>
       <c r="AA8">
@@ -888,9 +1045,9 @@
       <c r="AF8">
         <v>1</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AG8" s="3" t="e" vm="2">
         <f>-S4*$S$1*8.76</f>
-        <v>-0.74358288770053482</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -912,13 +1069,13 @@
       <c r="X9">
         <v>1</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="3" t="e" vm="2">
         <f>-Q5*$Q$1*8.76</f>
-        <v>-2.8282181000562119</v>
-      </c>
-      <c r="Z9" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="3" t="e" vm="2">
         <f>-R5*$Q$1*8.76</f>
-        <v>-6.7451999999999996</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -935,9 +1092,9 @@
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="3" t="e" vm="2">
         <f>-S5*$S$1*8.76</f>
-        <v>-0.40993272655322516</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI9">
         <v>0</v>
@@ -1109,7 +1266,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA33"/>
+  <dimension ref="A1:AA85"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -1153,10 +1310,64 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W1" t="s">
+        <v>78</v>
+      </c>
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1182,7 +1393,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1199,7 +1410,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1216,7 +1427,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1233,7 +1444,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1259,7 +1470,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1285,7 +1496,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1311,7 +1522,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1337,7 +1548,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1363,1365 +1574,1978 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
       </c>
       <c r="D14">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="E14">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F14">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="G14">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="H14">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="I14">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="J14">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="K14">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="L14">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="M14">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="N14">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="O14">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="P14">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="Q14">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="R14">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="S14">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="T14">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="U14">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="V14">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="W14">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X14">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="Y14">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="Z14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15">
         <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.65507145273127021</v>
-      </c>
-      <c r="E15">
-        <v>0.70855841068035541</v>
-      </c>
-      <c r="F15">
-        <v>0.6572836882190054</v>
-      </c>
-      <c r="G15">
-        <v>0.66795828727795103</v>
-      </c>
-      <c r="H15">
-        <v>0.62441319864710465</v>
-      </c>
-      <c r="I15">
-        <v>0.61153310682623163</v>
-      </c>
-      <c r="J15">
-        <v>0.57753151026969707</v>
-      </c>
-      <c r="K15">
-        <v>0.59143141855243575</v>
-      </c>
-      <c r="L15">
-        <v>0.57563238385156201</v>
-      </c>
-      <c r="M15">
-        <v>0.57671093237261395</v>
-      </c>
-      <c r="N15">
-        <v>0.54659134266267884</v>
-      </c>
-      <c r="O15">
-        <v>0.48959346018435024</v>
-      </c>
-      <c r="P15">
-        <v>0.47204644576248633</v>
-      </c>
-      <c r="Q15">
-        <v>0.46064340026918904</v>
-      </c>
-      <c r="R15">
-        <v>0.46706407389769605</v>
-      </c>
-      <c r="S15">
-        <v>0.48648885924182372</v>
-      </c>
-      <c r="T15">
-        <v>0.51708852636124003</v>
-      </c>
-      <c r="U15">
-        <v>0.51871573462922282</v>
-      </c>
-      <c r="V15">
-        <v>0.4969645862171681</v>
-      </c>
-      <c r="W15">
-        <v>0.49137811601855713</v>
-      </c>
-      <c r="X15">
-        <v>0.51787948529646377</v>
-      </c>
-      <c r="Y15">
-        <v>0.5341149748927575</v>
-      </c>
-      <c r="Z15">
-        <v>0.54240480484752174</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>69.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18">
+        <v>68.39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20">
+        <v>77.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22">
+        <v>66.41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24">
+        <v>61.91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26">
+        <v>60.33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28">
+        <v>63.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30">
+        <v>56.81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="K32">
+        <v>47.99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L34">
+        <v>25.93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M36">
+        <v>30.71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="N38">
+        <v>56.41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="O40">
+        <v>44.52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="P42">
+        <v>48.46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q44">
+        <v>67.19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="R46">
+        <v>64.06</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" t="s">
+        <v>86</v>
+      </c>
+      <c r="S48">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>85</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="T50">
+        <v>40.130000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="U52">
+        <v>62.97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="V54">
+        <v>57.67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="W56">
+        <v>45.04</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" t="s">
+        <v>85</v>
+      </c>
+      <c r="X57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="X58">
+        <v>44.89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y59">
+        <v>14.94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z62">
+        <v>50.34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>2000</v>
+      </c>
+      <c r="E66">
+        <v>2001</v>
+      </c>
+      <c r="F66">
+        <v>2002</v>
+      </c>
+      <c r="G66">
+        <v>2003</v>
+      </c>
+      <c r="H66">
+        <v>2004</v>
+      </c>
+      <c r="I66">
+        <v>2005</v>
+      </c>
+      <c r="J66">
+        <v>2006</v>
+      </c>
+      <c r="K66">
+        <v>2007</v>
+      </c>
+      <c r="L66">
+        <v>2008</v>
+      </c>
+      <c r="M66">
+        <v>2009</v>
+      </c>
+      <c r="N66">
+        <v>2010</v>
+      </c>
+      <c r="O66">
+        <v>2011</v>
+      </c>
+      <c r="P66">
+        <v>2012</v>
+      </c>
+      <c r="Q66">
+        <v>2013</v>
+      </c>
+      <c r="R66">
+        <v>2014</v>
+      </c>
+      <c r="S66">
+        <v>2015</v>
+      </c>
+      <c r="T66">
+        <v>2016</v>
+      </c>
+      <c r="U66">
+        <v>2017</v>
+      </c>
+      <c r="V66">
+        <v>2018</v>
+      </c>
+      <c r="W66">
+        <v>2019</v>
+      </c>
+      <c r="X66">
+        <v>2020</v>
+      </c>
+      <c r="Y66">
+        <v>2021</v>
+      </c>
+      <c r="Z66">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.65507145273127021</v>
+      </c>
+      <c r="E67">
+        <v>0.70855841068035541</v>
+      </c>
+      <c r="F67">
+        <v>0.6572836882190054</v>
+      </c>
+      <c r="G67">
+        <v>0.66795828727795103</v>
+      </c>
+      <c r="H67">
+        <v>0.62441319864710465</v>
+      </c>
+      <c r="I67">
+        <v>0.61153310682623163</v>
+      </c>
+      <c r="J67">
+        <v>0.57753151026969707</v>
+      </c>
+      <c r="K67">
+        <v>0.59143141855243575</v>
+      </c>
+      <c r="L67">
+        <v>0.57563238385156201</v>
+      </c>
+      <c r="M67">
+        <v>0.57671093237261395</v>
+      </c>
+      <c r="N67">
+        <v>0.54659134266267884</v>
+      </c>
+      <c r="O67">
+        <v>0.48959346018435024</v>
+      </c>
+      <c r="P67">
+        <v>0.47204644576248633</v>
+      </c>
+      <c r="Q67">
+        <v>0.46064340026918904</v>
+      </c>
+      <c r="R67">
+        <v>0.46706407389769605</v>
+      </c>
+      <c r="S67">
+        <v>0.48648885924182372</v>
+      </c>
+      <c r="T67">
+        <v>0.51708852636124003</v>
+      </c>
+      <c r="U67">
+        <v>0.51871573462922282</v>
+      </c>
+      <c r="V67">
+        <v>0.4969645862171681</v>
+      </c>
+      <c r="W67">
+        <v>0.49137811601855713</v>
+      </c>
+      <c r="X67">
+        <v>0.51787948529646377</v>
+      </c>
+      <c r="Y67">
+        <v>0.5341149748927575</v>
+      </c>
+      <c r="Z67">
+        <v>0.54240480484752174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" t="s">
         <v>12</v>
       </c>
-      <c r="O16">
+      <c r="O68">
         <v>0.47682418559038953</v>
       </c>
-      <c r="P16">
+      <c r="P68">
         <v>0.47787079316759684</v>
       </c>
-      <c r="Q16">
+      <c r="Q68">
         <v>0.68608066971080672</v>
       </c>
-      <c r="R16">
+      <c r="R68">
         <v>0.63251902587519038</v>
       </c>
-      <c r="S16">
+      <c r="S68">
         <v>0.71154709387818282</v>
       </c>
-      <c r="T16">
+      <c r="T68">
         <v>0.68991475465456553</v>
       </c>
-      <c r="U16">
+      <c r="U68">
         <v>0.94102096498296517</v>
       </c>
-      <c r="V16">
+      <c r="V68">
         <v>0.89751473769031775</v>
       </c>
-      <c r="W16">
+      <c r="W68">
         <v>0.90819514539774093</v>
       </c>
-      <c r="X16">
+      <c r="X68">
         <v>0.94150868710858548</v>
       </c>
-      <c r="Y16">
+      <c r="Y68">
         <v>0.70902073879299388</v>
       </c>
-      <c r="Z16">
+      <c r="Z68">
         <v>0.80293905593960735</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
         <v>13</v>
       </c>
-      <c r="D17">
+      <c r="D69">
         <v>0.32282078015860649</v>
       </c>
-      <c r="E17">
+      <c r="E69">
         <v>0.35595105709784614</v>
       </c>
-      <c r="F17">
+      <c r="F69">
         <v>0.29729053112042492</v>
       </c>
-      <c r="G17">
+      <c r="G69">
         <v>0.29083409798800802</v>
       </c>
-      <c r="H17">
+      <c r="H69">
         <v>0.29496174796927549</v>
       </c>
-      <c r="I17">
+      <c r="I69">
         <v>0.25589254143295048</v>
       </c>
-      <c r="J17">
+      <c r="J69">
         <v>0.28033326413732557</v>
       </c>
-      <c r="K17">
+      <c r="K69">
         <v>0.28707591471688315</v>
       </c>
-      <c r="L17">
+      <c r="L69">
         <v>0.31068978946717857</v>
       </c>
-      <c r="M17">
+      <c r="M69">
         <v>0.28061596014311618</v>
       </c>
-      <c r="N17">
+      <c r="N69">
         <v>0.30318205573739576</v>
       </c>
-      <c r="O17">
+      <c r="O69">
         <v>0.22657361497385858</v>
       </c>
-      <c r="P17">
+      <c r="P69">
         <v>0.28814545753169268</v>
       </c>
-      <c r="Q17">
+      <c r="Q69">
         <v>0.34306621642304425</v>
       </c>
-      <c r="R17">
+      <c r="R69">
         <v>0.31112192879741829</v>
       </c>
-      <c r="S17">
+      <c r="S69">
         <v>0.27034926347874866</v>
       </c>
-      <c r="T17">
+      <c r="T69">
         <v>0.2926659088325631</v>
       </c>
-      <c r="U17">
+      <c r="U69">
         <v>0.24483427383365902</v>
       </c>
-      <c r="V17">
+      <c r="V69">
         <v>0.31269804580294608</v>
       </c>
-      <c r="W17">
+      <c r="W69">
         <v>0.27171404276150501</v>
       </c>
-      <c r="X17">
+      <c r="X69">
         <v>0.29510118752862963</v>
       </c>
-      <c r="Y17">
+      <c r="Y69">
         <v>0.28086313296037818</v>
       </c>
-      <c r="Z17">
+      <c r="Z69">
         <v>0.22444913497305133</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" t="s">
         <v>14</v>
       </c>
-      <c r="D18">
+      <c r="D70">
         <v>0.75008977690880807</v>
       </c>
-      <c r="E18">
+      <c r="E70">
         <v>0.76077483705554294</v>
       </c>
-      <c r="F18">
+      <c r="F70">
         <v>0.7879893080553233</v>
       </c>
-      <c r="G18">
+      <c r="G70">
         <v>0.79463498604871241</v>
       </c>
-      <c r="H18">
+      <c r="H70">
         <v>0.8075543128788194</v>
       </c>
-      <c r="I18">
+      <c r="I70">
         <v>0.8148025038364537</v>
       </c>
-      <c r="J18">
+      <c r="J70">
         <v>0.81238802824322898</v>
       </c>
-      <c r="K18">
+      <c r="K70">
         <v>0.79351072691234414</v>
       </c>
-      <c r="L18">
+      <c r="L70">
         <v>0.79300004186534656</v>
       </c>
-      <c r="M18">
+      <c r="M70">
         <v>0.74090790403508877</v>
       </c>
-      <c r="N18">
+      <c r="N70">
         <v>0.77487600783192179</v>
       </c>
-      <c r="O18">
+      <c r="O70">
         <v>0.79995067617954385</v>
       </c>
-      <c r="P18">
+      <c r="P70">
         <v>0.76924331867198725</v>
       </c>
-      <c r="Q18">
+      <c r="Q70">
         <v>0.76613068307985177</v>
       </c>
-      <c r="R18">
+      <c r="R70">
         <v>0.78926613163964765</v>
       </c>
-      <c r="S18">
+      <c r="S70">
         <v>0.79098180387357531</v>
       </c>
-      <c r="T18">
+      <c r="T70">
         <v>0.72908096795262656</v>
       </c>
-      <c r="U18">
+      <c r="U70">
         <v>0.72033559980239359</v>
       </c>
-      <c r="V18">
+      <c r="V70">
         <v>0.74670483535098608</v>
       </c>
-      <c r="W18">
+      <c r="W70">
         <v>0.72151541141096831</v>
       </c>
-      <c r="X18">
+      <c r="X70">
         <v>0.65784820512248465</v>
       </c>
-      <c r="Y18">
+      <c r="Y70">
         <v>0.70531080719289641</v>
       </c>
-      <c r="Z18">
+      <c r="Z70">
         <v>0.54796572739577298</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="D71">
         <v>3.6927707854271789E-2</v>
       </c>
-      <c r="E19">
+      <c r="E71">
         <v>3.2106164383561647E-2</v>
       </c>
-      <c r="F19">
+      <c r="F71">
         <v>3.0674905885911357E-2</v>
       </c>
-      <c r="G19">
+      <c r="G71">
         <v>3.723476881607915E-2</v>
       </c>
-      <c r="H19">
+      <c r="H71">
         <v>3.5518030365180489E-2</v>
       </c>
-      <c r="I19">
+      <c r="I71">
         <v>4.2416457904387937E-2</v>
       </c>
-      <c r="J19">
+      <c r="J71">
         <v>3.9887577105863672E-2</v>
       </c>
-      <c r="K19">
+      <c r="K71">
         <v>3.815298856026976E-2</v>
       </c>
-      <c r="L19">
+      <c r="L71">
         <v>3.4664567786608445E-2</v>
       </c>
-      <c r="M19">
+      <c r="M71">
         <v>3.0554855784857463E-2</v>
       </c>
-      <c r="N19">
+      <c r="N71">
         <v>3.1924978980746692E-2</v>
       </c>
-      <c r="O19">
+      <c r="O71">
         <v>4.2420421651444461E-2</v>
       </c>
-      <c r="P19">
+      <c r="P71">
         <v>4.4328624511802063E-2</v>
       </c>
-      <c r="Q19">
+      <c r="Q71">
         <v>4.3455693252832557E-2</v>
       </c>
-      <c r="R19">
+      <c r="R71">
         <v>4.654041069231591E-2</v>
       </c>
-      <c r="S19">
+      <c r="S71">
         <v>4.4431352478279694E-2</v>
       </c>
-      <c r="T19">
+      <c r="T71">
         <v>4.8236179261924875E-2</v>
       </c>
-      <c r="U19">
+      <c r="U71">
         <v>5.73174118940072E-2</v>
       </c>
-      <c r="V19">
+      <c r="V71">
         <v>5.2895430041181767E-2</v>
       </c>
-      <c r="W19">
+      <c r="W71">
         <v>5.3900035971085496E-2</v>
       </c>
-      <c r="X19">
+      <c r="X71">
         <v>5.1096165415330838E-2</v>
       </c>
-      <c r="Y19">
+      <c r="Y71">
         <v>5.0187342643328442E-2</v>
       </c>
-      <c r="Z19">
+      <c r="Z71">
         <v>4.9969373471372251E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" t="s">
         <v>15</v>
       </c>
-      <c r="D20">
+      <c r="D72">
         <v>8.51761252446184E-2</v>
       </c>
-      <c r="E20">
+      <c r="E72">
         <v>0.10047292889758642</v>
       </c>
-      <c r="F20">
+      <c r="F72">
         <v>0.10136986301369863</v>
       </c>
-      <c r="G20">
+      <c r="G72">
         <v>9.8515981735159838E-2</v>
       </c>
-      <c r="H20">
+      <c r="H72">
         <v>8.7671232876712343E-2</v>
       </c>
-      <c r="I20">
+      <c r="I72">
         <v>9.2211099402880234E-2</v>
       </c>
-      <c r="J20">
+      <c r="J72">
         <v>9.2108066971080677E-2</v>
       </c>
-      <c r="K20">
+      <c r="K72">
         <v>7.7151387425360041E-2</v>
       </c>
-      <c r="L20">
+      <c r="L72">
         <v>5.9492009132420094E-2</v>
       </c>
-      <c r="M20">
+      <c r="M72">
         <v>7.1695679409195065E-2</v>
       </c>
-      <c r="N20">
+      <c r="N72">
         <v>6.7793348379082907E-2</v>
       </c>
-      <c r="O20">
+      <c r="O72">
         <v>8.9144951765142907E-2</v>
       </c>
-      <c r="P20">
+      <c r="P72">
         <v>0.11753105059980719</v>
       </c>
-      <c r="Q20">
+      <c r="Q72">
         <v>0.11489224215382465</v>
       </c>
-      <c r="R20">
+      <c r="R72">
         <v>0.12448158526861221</v>
       </c>
-      <c r="S20">
+      <c r="S72">
         <v>0.12979460687322764</v>
       </c>
-      <c r="T20">
+      <c r="T72">
         <v>0.13506891572810997</v>
       </c>
-      <c r="U20">
+      <c r="U72">
         <v>0.13509952073241918</v>
       </c>
-      <c r="V20">
+      <c r="V72">
         <v>0.13660941729581461</v>
       </c>
-      <c r="W20">
+      <c r="W72">
         <v>0.13869028839168057</v>
       </c>
-      <c r="X20">
+      <c r="X72">
         <v>0.1352356616976321</v>
       </c>
-      <c r="Y20">
+      <c r="Y72">
         <v>0.13037828662205719</v>
       </c>
-      <c r="Z20">
+      <c r="Z72">
         <v>0.15496417492770403</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" t="s">
         <v>16</v>
       </c>
-      <c r="D21">
+      <c r="D73">
         <v>0.14467676039413602</v>
       </c>
-      <c r="E21">
+      <c r="E73">
         <v>0.22699598726995987</v>
       </c>
-      <c r="F21">
+      <c r="F73">
         <v>0.21969922572960091</v>
       </c>
-      <c r="G21">
+      <c r="G73">
         <v>0.20304448912906872</v>
       </c>
-      <c r="H21">
+      <c r="H73">
         <v>0.18967947246243719</v>
       </c>
-      <c r="I21">
+      <c r="I73">
         <v>0.15924988419032496</v>
       </c>
-      <c r="J21">
+      <c r="J73">
         <v>0.17645394336864709</v>
       </c>
-      <c r="K21">
+      <c r="K73">
         <v>0.20900784040654269</v>
       </c>
-      <c r="L21">
+      <c r="L73">
         <v>0.19101497872545981</v>
       </c>
-      <c r="M21">
+      <c r="M73">
         <v>0.19710765174028208</v>
       </c>
-      <c r="N21">
+      <c r="N73">
         <v>0.19202855734949736</v>
       </c>
-      <c r="O21">
+      <c r="O73">
         <v>0.20897927349870182</v>
       </c>
-      <c r="P21">
+      <c r="P73">
         <v>0.22776141636182795</v>
       </c>
-      <c r="Q21">
+      <c r="Q73">
         <v>0.2257468487267531</v>
       </c>
-      <c r="R21">
+      <c r="R73">
         <v>0.21492394513606378</v>
       </c>
-      <c r="S21">
+      <c r="S73">
         <v>0.23744797980775009</v>
       </c>
-      <c r="T21">
+      <c r="T73">
         <v>0.21101790768326553</v>
       </c>
-      <c r="U21">
+      <c r="U73">
         <v>0.20810602325113201</v>
       </c>
-      <c r="V21">
+      <c r="V73">
         <v>0.21910392366842035</v>
       </c>
-      <c r="W21">
+      <c r="W73">
         <v>0.24129166336449459</v>
       </c>
-      <c r="X21">
+      <c r="X73">
         <v>0.26069700487040792</v>
       </c>
-      <c r="Y21">
+      <c r="Y73">
         <v>0.22841616489062896</v>
       </c>
-      <c r="Z21">
+      <c r="Z73">
         <v>0.20822393273037404</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B77" t="s">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C77" t="s">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="D77">
         <v>2000</v>
       </c>
-      <c r="E25">
+      <c r="E77">
         <v>2001</v>
       </c>
-      <c r="F25">
+      <c r="F77">
         <v>2002</v>
       </c>
-      <c r="G25">
+      <c r="G77">
         <v>2003</v>
       </c>
-      <c r="H25">
+      <c r="H77">
         <v>2004</v>
       </c>
-      <c r="I25">
+      <c r="I77">
         <v>2005</v>
       </c>
-      <c r="J25">
+      <c r="J77">
         <v>2006</v>
       </c>
-      <c r="K25">
+      <c r="K77">
         <v>2007</v>
       </c>
-      <c r="L25">
+      <c r="L77">
         <v>2008</v>
       </c>
-      <c r="M25">
+      <c r="M77">
         <v>2009</v>
       </c>
-      <c r="N25">
+      <c r="N77">
         <v>2010</v>
       </c>
-      <c r="O25">
+      <c r="O77">
         <v>2011</v>
       </c>
-      <c r="P25">
+      <c r="P77">
         <v>2012</v>
       </c>
-      <c r="Q25">
+      <c r="Q77">
         <v>2013</v>
       </c>
-      <c r="R25">
+      <c r="R77">
         <v>2014</v>
       </c>
-      <c r="S25">
+      <c r="S77">
         <v>2015</v>
       </c>
-      <c r="T25">
+      <c r="T77">
         <v>2016</v>
       </c>
-      <c r="U25">
+      <c r="U77">
         <v>2017</v>
       </c>
-      <c r="V25">
+      <c r="V77">
         <v>2018</v>
       </c>
-      <c r="W25">
+      <c r="W77">
         <v>2019</v>
       </c>
-      <c r="X25">
+      <c r="X77">
         <v>2020</v>
       </c>
-      <c r="Y25">
+      <c r="Y77">
         <v>2021</v>
       </c>
-      <c r="Z25">
+      <c r="Z77">
         <v>2022</v>
       </c>
-      <c r="AA25">
+      <c r="AA77">
         <v>2023</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" t="s">
         <v>0</v>
       </c>
-      <c r="D26">
+      <c r="D78">
         <v>0.52511415525114158</v>
       </c>
-      <c r="E26">
+      <c r="E78">
         <v>0.56736863627070133</v>
       </c>
-      <c r="F26">
+      <c r="F78">
         <v>0.53729071537290718</v>
       </c>
-      <c r="G26">
+      <c r="G78">
         <v>0.55150329122931863</v>
       </c>
-      <c r="H26">
+      <c r="H78">
         <v>0.5198877702591187</v>
       </c>
-      <c r="I26">
+      <c r="I78">
         <v>0.52592954990215257</v>
       </c>
-      <c r="J26">
+      <c r="J78">
         <v>0.4981320049813201</v>
       </c>
-      <c r="K26">
+      <c r="K78">
         <v>0.51248421257165067</v>
       </c>
-      <c r="L26">
+      <c r="L78">
         <v>0.50183100501831013</v>
       </c>
-      <c r="M26">
+      <c r="M78">
         <v>0.50272216368106781</v>
       </c>
-      <c r="N26">
+      <c r="N78">
         <v>0.4926700312424897</v>
       </c>
-      <c r="O26">
+      <c r="O78">
         <v>0.45499021526418787</v>
       </c>
-      <c r="P26">
+      <c r="P78">
         <v>0.43923311863074177</v>
       </c>
-      <c r="Q26">
+      <c r="Q78">
         <v>0.43017039759438686</v>
       </c>
-      <c r="R26">
+      <c r="R78">
         <v>0.43983346763362885</v>
       </c>
-      <c r="S26">
+      <c r="S78">
         <v>0.4585558393313211</v>
       </c>
-      <c r="T26">
+      <c r="T78">
         <v>0.48786349435231918</v>
       </c>
-      <c r="U26">
+      <c r="U78">
         <v>0.49350193185809621</v>
       </c>
-      <c r="V26">
+      <c r="V78">
         <v>0.47511838322340605</v>
       </c>
-      <c r="W26">
+      <c r="W78">
         <v>0.47140003261578606</v>
       </c>
-      <c r="X26">
+      <c r="X78">
         <v>0.49520125147979022</v>
       </c>
-      <c r="Y26">
+      <c r="Y78">
         <v>0.51042986743910046</v>
       </c>
-      <c r="Z26">
+      <c r="Z78">
         <v>0.51743733923550872</v>
       </c>
-      <c r="AA26">
+      <c r="AA78">
         <v>0.47840997366376781</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D79">
         <v>0.36692759295499022</v>
       </c>
-      <c r="E27">
+      <c r="E79">
         <v>0.27832137421178516</v>
       </c>
-      <c r="F27">
+      <c r="F79">
         <v>0.3215372907153729</v>
       </c>
-      <c r="G27">
+      <c r="G79">
         <v>0.35687105892585347</v>
       </c>
-      <c r="H27">
+      <c r="H79">
         <v>0.32922644619167279</v>
       </c>
-      <c r="I27">
+      <c r="I79">
         <v>0.40678898431400384</v>
       </c>
-      <c r="J27">
+      <c r="J79">
         <v>0.34701377139842454</v>
       </c>
-      <c r="K27">
+      <c r="K79">
         <v>0.37066346486201313</v>
       </c>
-      <c r="L27">
+      <c r="L79">
         <v>0.3450091862810224</v>
       </c>
-      <c r="M27">
+      <c r="M79">
         <v>0.32421288233780388</v>
       </c>
-      <c r="N27">
+      <c r="N79">
         <v>0.34949759720401924</v>
       </c>
-      <c r="O27">
+      <c r="O79">
         <v>0.26017821983638251</v>
       </c>
-      <c r="P27">
+      <c r="P79">
         <v>0.31009768221490086</v>
       </c>
-      <c r="Q27">
+      <c r="Q79">
         <v>0.43129337356808434</v>
       </c>
-      <c r="R27">
+      <c r="R79">
         <v>0.2216186427334278</v>
       </c>
-      <c r="S27">
+      <c r="S79">
         <v>0.36291602568798381</v>
       </c>
-      <c r="T27">
+      <c r="T79">
         <v>0.31224818694601131</v>
       </c>
-      <c r="U27">
+      <c r="U79">
         <v>0.3909969965570288</v>
       </c>
-      <c r="V27">
+      <c r="V79">
         <v>0.25364442165409129</v>
       </c>
-      <c r="W27">
+      <c r="W79">
         <v>0.11110297169926502</v>
       </c>
-      <c r="X27">
+      <c r="X79">
         <v>9.4315434766683762E-2</v>
       </c>
-      <c r="Y27">
+      <c r="Y79">
         <v>0.19967992482638128</v>
       </c>
-      <c r="Z27">
+      <c r="Z79">
         <v>0.19692917826411252</v>
       </c>
-      <c r="AA27">
+      <c r="AA79">
         <v>9.8237188233367925E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>47</v>
       </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B80" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" t="s">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="D80">
         <v>5.1995525945360881E-2</v>
       </c>
-      <c r="E28">
+      <c r="E80">
         <v>6.6085290592071855E-2</v>
       </c>
-      <c r="F28">
+      <c r="F80">
         <v>7.7927609196221478E-2</v>
       </c>
-      <c r="G28">
+      <c r="G80">
         <v>8.3409551663971043E-2</v>
       </c>
-      <c r="H28">
+      <c r="H80">
         <v>9.1821476367202157E-2</v>
       </c>
-      <c r="I28">
+      <c r="I80">
         <v>0.10347982883440537</v>
       </c>
-      <c r="J28">
+      <c r="J80">
         <v>0.10081242957955287</v>
       </c>
-      <c r="K28">
+      <c r="K80">
         <v>0.10300672846133523</v>
       </c>
-      <c r="L28">
+      <c r="L80">
         <v>0.10308365228960664</v>
       </c>
-      <c r="M28">
+      <c r="M80">
         <v>9.0634494515949904E-2</v>
       </c>
-      <c r="N28">
+      <c r="N80">
         <v>0.1003822637721424</v>
       </c>
-      <c r="O28">
+      <c r="O80">
         <v>0.12589522648333523</v>
       </c>
-      <c r="P28">
+      <c r="P80">
         <v>9.3789525585782574E-2</v>
       </c>
-      <c r="Q28">
+      <c r="Q80">
         <v>8.2261562245029424E-2</v>
       </c>
-      <c r="R28">
+      <c r="R80">
         <v>6.3254025474645523E-2</v>
       </c>
-      <c r="S28">
+      <c r="S80">
         <v>0.10199670368268894</v>
       </c>
-      <c r="T28">
+      <c r="T80">
         <v>0.17702922981907276</v>
       </c>
-      <c r="U28">
+      <c r="U80">
         <v>0.23684875364922525</v>
       </c>
-      <c r="V28">
+      <c r="V80">
         <v>0.18576779571732707</v>
       </c>
-      <c r="W28">
+      <c r="W80">
         <v>0.26227018833281296</v>
       </c>
-      <c r="X28">
+      <c r="X80">
         <v>0.23139577934098482</v>
       </c>
-      <c r="Y28">
+      <c r="Y80">
         <v>0.22030309046390048</v>
       </c>
-      <c r="Z28">
+      <c r="Z80">
         <v>0.29350540681363757</v>
       </c>
-      <c r="AA28">
+      <c r="AA80">
         <v>0.19394051585832409</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
         <v>13</v>
       </c>
-      <c r="D29">
+      <c r="D81">
         <v>0.31738099437552669</v>
       </c>
-      <c r="E29">
+      <c r="E81">
         <v>0.35548689270581235</v>
       </c>
-      <c r="F29">
+      <c r="F81">
         <v>0.28699663480848048</v>
       </c>
-      <c r="G29">
+      <c r="G81">
         <v>0.27941970349842243</v>
       </c>
-      <c r="H29">
+      <c r="H81">
         <v>0.28411538491662558</v>
       </c>
-      <c r="I29">
+      <c r="I81">
         <v>0.24533837514948323</v>
       </c>
-      <c r="J29">
+      <c r="J81">
         <v>0.26841646026771221</v>
       </c>
-      <c r="K29">
+      <c r="K81">
         <v>0.27372815894713171</v>
       </c>
-      <c r="L29">
+      <c r="L81">
         <v>0.30441400304414001</v>
       </c>
-      <c r="M29">
+      <c r="M81">
         <v>0.27070405495063032</v>
       </c>
-      <c r="N29">
+      <c r="N81">
         <v>0.29577905884263395</v>
       </c>
-      <c r="O29">
+      <c r="O81">
         <v>0.21911293274085661</v>
       </c>
-      <c r="P29">
+      <c r="P81">
         <v>0.2863693365114921</v>
       </c>
-      <c r="Q29">
+      <c r="Q81">
         <v>0.34438110998743526</v>
       </c>
-      <c r="R29">
+      <c r="R81">
         <v>0.30586892291163043</v>
       </c>
-      <c r="S29">
+      <c r="S81">
         <v>0.26626640442588823</v>
       </c>
-      <c r="T29">
+      <c r="T81">
         <v>0.29071601002310821</v>
       </c>
-      <c r="U29">
+      <c r="U81">
         <v>0.23802179137104362</v>
       </c>
-      <c r="V29">
+      <c r="V81">
         <v>0.30969368340943682</v>
       </c>
-      <c r="W29">
+      <c r="W81">
         <v>0.2691207681220279</v>
       </c>
-      <c r="X29">
+      <c r="X81">
         <v>0.29488143495459235</v>
       </c>
-      <c r="Y29">
+      <c r="Y81">
         <v>0.28054147044762406</v>
       </c>
-      <c r="Z29">
+      <c r="Z81">
         <v>0.21437075214370757</v>
       </c>
-      <c r="AA29">
+      <c r="AA81">
         <v>0.25152932097013991</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
         <v>47</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" t="s">
         <v>14</v>
       </c>
-      <c r="D30">
+      <c r="D82">
         <v>0.75012178005582386</v>
       </c>
-      <c r="E30">
+      <c r="E82">
         <v>0.76081818851986283</v>
       </c>
-      <c r="F30">
+      <c r="F82">
         <v>0.78802667122782466</v>
       </c>
-      <c r="G30">
+      <c r="G82">
         <v>0.79467261081130947</v>
       </c>
-      <c r="H30">
+      <c r="H82">
         <v>0.80759074765924088</v>
       </c>
-      <c r="I30">
+      <c r="I82">
         <v>0.81480430837725581</v>
       </c>
-      <c r="J30">
+      <c r="J82">
         <v>0.81238622370242686</v>
       </c>
-      <c r="K30">
+      <c r="K82">
         <v>0.79351072691234414</v>
       </c>
-      <c r="L30">
+      <c r="L82">
         <v>0.79300545548775292</v>
       </c>
-      <c r="M30">
+      <c r="M82">
         <v>0.7409151370622481</v>
       </c>
-      <c r="N30">
+      <c r="N82">
         <v>0.77487419957513193</v>
       </c>
-      <c r="O30">
+      <c r="O82">
         <v>0.79995472124998268</v>
       </c>
-      <c r="P30">
+      <c r="P82">
         <v>0.7692505209587811</v>
       </c>
-      <c r="Q30">
+      <c r="Q82">
         <v>0.76612223671238655</v>
       </c>
-      <c r="R30">
+      <c r="R82">
         <v>0.78926792362212639</v>
       </c>
-      <c r="S30">
+      <c r="S82">
         <v>0.79098576757245864</v>
       </c>
-      <c r="T30">
+      <c r="T82">
         <v>0.72908913765680294</v>
       </c>
-      <c r="U30">
+      <c r="U82">
         <v>0.72033717479405757</v>
       </c>
-      <c r="V30">
+      <c r="V82">
         <v>0.74670155878968303</v>
       </c>
-      <c r="W30">
+      <c r="W82">
         <v>0.72151254170744272</v>
       </c>
-      <c r="X30">
+      <c r="X82">
         <v>0.65784287477875458</v>
       </c>
-      <c r="Y30">
+      <c r="Y82">
         <v>0.70530840509868675</v>
       </c>
-      <c r="Z30">
+      <c r="Z82">
         <v>0.54796379753989866</v>
       </c>
-      <c r="AA30">
+      <c r="AA82">
         <v>0.62404250888700497</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
         <v>3</v>
       </c>
-      <c r="D31">
+      <c r="D83">
         <v>1.4347239518472397</v>
       </c>
-      <c r="E31">
+      <c r="E83">
         <v>1.2712743877127439</v>
       </c>
-      <c r="F31">
+      <c r="F83">
         <v>1.266085512660855</v>
       </c>
-      <c r="G31">
+      <c r="G83">
         <v>1.4217517642175177</v>
       </c>
-      <c r="H31">
+      <c r="H83">
         <v>1.2681159420289856</v>
       </c>
-      <c r="I31">
+      <c r="I83">
         <v>1.4951856263648997</v>
       </c>
-      <c r="J31">
+      <c r="J83">
         <v>1.4331447290053603</v>
       </c>
-      <c r="K31">
+      <c r="K83">
         <v>1.2480242360379346</v>
       </c>
-      <c r="L31">
+      <c r="L83">
         <v>0.7913735653461681</v>
       </c>
-      <c r="M31">
+      <c r="M83">
         <v>0.59863557295064151</v>
       </c>
-      <c r="N31">
+      <c r="N83">
         <v>0.66634809387278326</v>
       </c>
-      <c r="O31">
+      <c r="O83">
         <v>0.80505999787618143</v>
       </c>
-      <c r="P31">
+      <c r="P83">
         <v>0.84355421047042589</v>
       </c>
-      <c r="Q31">
+      <c r="Q83">
         <v>0.75727407879367103</v>
       </c>
-      <c r="R31">
+      <c r="R83">
         <v>0.69974083672713816</v>
       </c>
-      <c r="S31">
+      <c r="S83">
         <v>0.71331932062525671</v>
       </c>
-      <c r="T31">
+      <c r="T83">
         <v>0.68855548307603109</v>
       </c>
-      <c r="U31">
+      <c r="U83">
         <v>0.73204319779662241</v>
       </c>
-      <c r="V31">
+      <c r="V83">
         <v>0.63781981590200776</v>
       </c>
-      <c r="W31">
+      <c r="W83">
         <v>0.64687975646879758</v>
       </c>
-      <c r="X31">
+      <c r="X83">
         <v>0.59019441698441844</v>
       </c>
-      <c r="Y31">
+      <c r="Y83">
         <v>0.59195970437320533</v>
       </c>
-      <c r="Z31">
+      <c r="Z83">
         <v>0.61490844042743487</v>
       </c>
-      <c r="AA31">
+      <c r="AA83">
         <v>0.57136468483735825</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
         <v>47</v>
       </c>
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" t="s">
         <v>15</v>
       </c>
-      <c r="D32">
+      <c r="D84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="E32">
+      <c r="E84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="F32">
+      <c r="F84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="G32">
+      <c r="G84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="H32">
+      <c r="H84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="I32">
+      <c r="I84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="J32">
+      <c r="J84">
         <v>0.11415525114155252</v>
       </c>
-      <c r="K32">
+      <c r="K84">
         <v>7.6103500761035017E-2</v>
       </c>
-      <c r="L32">
+      <c r="L84">
         <v>5.7077625570776259E-2</v>
       </c>
-      <c r="M32">
+      <c r="M84">
         <v>6.9308545335942592E-2</v>
       </c>
-      <c r="N32">
+      <c r="N84">
         <v>6.8054092026694768E-2</v>
       </c>
-      <c r="O32">
+      <c r="O84">
         <v>8.8660578386605779E-2</v>
       </c>
-      <c r="P32">
+      <c r="P84">
         <v>0.11598801893510953</v>
       </c>
-      <c r="Q32">
+      <c r="Q84">
         <v>0.11220942299709424</v>
       </c>
-      <c r="R32">
+      <c r="R84">
         <v>0.12097049001567504</v>
       </c>
-      <c r="S32">
+      <c r="S84">
         <v>0.12390801069286163</v>
       </c>
-      <c r="T32">
+      <c r="T84">
         <v>0.1283875941410188</v>
       </c>
-      <c r="U32">
+      <c r="U84">
         <v>0.1271485317592902</v>
       </c>
-      <c r="V32">
+      <c r="V84">
         <v>0.12814312199794212</v>
       </c>
-      <c r="W32">
+      <c r="W84">
         <v>0.12935469333265309</v>
       </c>
-      <c r="X32">
+      <c r="X84">
         <v>0.12621188286312468</v>
       </c>
-      <c r="Y32">
+      <c r="Y84">
         <v>0.12001537697017431</v>
       </c>
-      <c r="Z32">
+      <c r="Z84">
         <v>0.12915663284776227</v>
       </c>
-      <c r="AA32">
+      <c r="AA84">
         <v>0.1291537512915375</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
         <v>47</v>
       </c>
-      <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B85" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" t="s">
         <v>16</v>
       </c>
-      <c r="D33">
+      <c r="D85">
         <v>0.14269406392694065</v>
       </c>
-      <c r="E33">
+      <c r="E85">
         <v>0.21200260926288322</v>
       </c>
-      <c r="F33">
+      <c r="F85">
         <v>0.22015655577299412</v>
       </c>
-      <c r="G33">
+      <c r="G85">
         <v>0.20236612702366127</v>
       </c>
-      <c r="H33">
+      <c r="H85">
         <v>0.18708777270421106</v>
       </c>
-      <c r="I33">
+      <c r="I85">
         <v>0.15882469724042089</v>
       </c>
-      <c r="J33">
+      <c r="J85">
         <v>0.17649535282878334</v>
       </c>
-      <c r="K33">
+      <c r="K85">
         <v>0.20928462709284626</v>
       </c>
-      <c r="L33">
+      <c r="L85">
         <v>0.19104217029277468</v>
       </c>
-      <c r="M33">
+      <c r="M85">
         <v>0.19715459312875117</v>
       </c>
-      <c r="N33">
+      <c r="N85">
         <v>0.19199715674230658</v>
       </c>
-      <c r="O33">
+      <c r="O85">
         <v>0.20889060009186458</v>
       </c>
-      <c r="P33">
+      <c r="P85">
         <v>0.22771047468183536</v>
       </c>
-      <c r="Q33">
+      <c r="Q85">
         <v>0.22565247560211299</v>
       </c>
-      <c r="R33">
+      <c r="R85">
         <v>0.21490966845344453</v>
       </c>
-      <c r="S33">
+      <c r="S85">
         <v>0.23739859023806356</v>
       </c>
-      <c r="T33">
+      <c r="T85">
         <v>0.21094548568767438</v>
       </c>
-      <c r="U33">
+      <c r="U85">
         <v>0.20810079485878574</v>
       </c>
-      <c r="V33">
+      <c r="V85">
         <v>0.21911679078177193</v>
       </c>
-      <c r="W33">
+      <c r="W85">
         <v>0.24123373826139399</v>
       </c>
-      <c r="X33">
+      <c r="X85">
         <v>0.259420086117576</v>
       </c>
-      <c r="Y33">
+      <c r="Y85">
         <v>0.22664894337161073</v>
       </c>
-      <c r="Z33">
+      <c r="Z85">
         <v>0.21152457876108918</v>
       </c>
-      <c r="AA33">
+      <c r="AA85">
         <v>0.24995886297256162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 07:03
</commit_message>
<xml_diff>
--- a/VerveStacks_FRA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_FRA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FRA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF91F2B6-BBB7-40FA-949A-4FD02B626781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC2A970-A75D-4CEB-B831-854BEB2094E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -300,16 +300,53 @@
   </si>
   <si>
     <t>geothermal</t>
+  </si>
+  <si>
+    <t>VERVESTACKS: the open USE platform. Powered by data | Guided by intuition | Built with AI.</t>
+  </si>
+  <si>
+    <t>EMBER Utilization Factors</t>
+  </si>
+  <si>
+    <t>IRENA Utilization Factors</t>
+  </si>
+  <si>
+    <t>EMBER Capacity (GW)</t>
+  </si>
+  <si>
+    <t>EMBER Generation (TWh)</t>
+  </si>
+  <si>
+    <t>IRENA Generation (TWh)</t>
+  </si>
+  <si>
+    <t>IRENA Capacity (GW)</t>
+  </si>
+  <si>
+    <t>Electricity Trade Data (TWh) - Source: EMBER (estimated)</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Export</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,8 +380,35 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF969696"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +421,26 @@
         <bgColor rgb="FFDCE6F1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF19375F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F9FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -366,12 +448,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,6 +494,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,9 +1533,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A84"/>
+  <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Z88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1427,14 +1554,4300 @@
     <col min="26" max="27" width="4.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="15" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+    </row>
+    <row r="2" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K3" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O3" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P3" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R3" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S3" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T3" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U3" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V3" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W3" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X3" s="10">
+        <v>2022</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.52511415525114158</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.56736863627070133</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.53729071537290718</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.55150329122931863</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.5198877702591187</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.52592954990215257</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.4981320049813201</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.51248421257165067</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.50183100501831013</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.50272216368106781</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0.4926700312424897</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0.45499021526418787</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.43923311863074177</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.43017039759438686</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.43983346763362885</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>0.4585558393313211</v>
+      </c>
+      <c r="R4" s="12">
+        <v>0.48786349435231918</v>
+      </c>
+      <c r="S4" s="12">
+        <v>0.49350193185809621</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0.47511838322340605</v>
+      </c>
+      <c r="U4" s="12">
+        <v>0.47140003261578606</v>
+      </c>
+      <c r="V4" s="12">
+        <v>0.49520125147979022</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0.51042986743910046</v>
+      </c>
+      <c r="X4" s="12">
+        <v>0.51743733923550872</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>0.47840997366376781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.36692759295499022</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.27832137421178516</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.3215372907153729</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.35687105892585347</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.32922644619167279</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.40678898431400384</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.34701377139842454</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0.37066346486201313</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.3450091862810224</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.32421288233780388</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0.34949759720401924</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0.26017821983638251</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.31009768221490086</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0.43129337356808434</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0.2216186427334278</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0.36291602568798381</v>
+      </c>
+      <c r="R5" s="14">
+        <v>0.31224818694601131</v>
+      </c>
+      <c r="S5" s="14">
+        <v>0.3909969965570288</v>
+      </c>
+      <c r="T5" s="14">
+        <v>0.25364442165409129</v>
+      </c>
+      <c r="U5" s="14">
+        <v>0.11110297169926502</v>
+      </c>
+      <c r="V5" s="14">
+        <v>9.4315434766683762E-2</v>
+      </c>
+      <c r="W5" s="14">
+        <v>0.19967992482638128</v>
+      </c>
+      <c r="X5" s="14">
+        <v>0.19692917826411252</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>9.8237188233367925E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12">
+        <v>5.1995525945360881E-2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>6.6085290592071855E-2</v>
+      </c>
+      <c r="D6" s="12">
+        <v>7.7927609196221478E-2</v>
+      </c>
+      <c r="E6" s="12">
+        <v>8.3409551663971043E-2</v>
+      </c>
+      <c r="F6" s="12">
+        <v>9.1821476367202157E-2</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.10347982883440537</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.10081242957955287</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.10300672846133523</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0.10308365228960664</v>
+      </c>
+      <c r="K6" s="12">
+        <v>9.0634494515949904E-2</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0.1003822637721424</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0.12589522648333523</v>
+      </c>
+      <c r="N6" s="12">
+        <v>9.3789525585782574E-2</v>
+      </c>
+      <c r="O6" s="12">
+        <v>8.2261562245029424E-2</v>
+      </c>
+      <c r="P6" s="12">
+        <v>6.3254025474645523E-2</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0.10199670368268894</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0.17702922981907276</v>
+      </c>
+      <c r="S6" s="12">
+        <v>0.23684875364922525</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0.18576779571732707</v>
+      </c>
+      <c r="U6" s="12">
+        <v>0.26227018833281296</v>
+      </c>
+      <c r="V6" s="12">
+        <v>0.23139577934098482</v>
+      </c>
+      <c r="W6" s="12">
+        <v>0.22030309046390048</v>
+      </c>
+      <c r="X6" s="12">
+        <v>0.29350540681363757</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>0.19394051585832409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.31738099437552669</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0.35548689270581235</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.28699663480848048</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.27941970349842243</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.28411538491662558</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0.24533837514948323</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.26841646026771221</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.27372815894713171</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.30441400304414001</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0.27070405495063032</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0.29577905884263395</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0.21911293274085661</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0.2863693365114921</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0.34438110998743526</v>
+      </c>
+      <c r="P7" s="14">
+        <v>0.30586892291163043</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>0.26626640442588823</v>
+      </c>
+      <c r="R7" s="14">
+        <v>0.29071601002310821</v>
+      </c>
+      <c r="S7" s="14">
+        <v>0.23802179137104362</v>
+      </c>
+      <c r="T7" s="14">
+        <v>0.30969368340943682</v>
+      </c>
+      <c r="U7" s="14">
+        <v>0.2691207681220279</v>
+      </c>
+      <c r="V7" s="14">
+        <v>0.29488143495459235</v>
+      </c>
+      <c r="W7" s="14">
+        <v>0.28054147044762406</v>
+      </c>
+      <c r="X7" s="14">
+        <v>0.21437075214370757</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>0.25152932097013991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.75012178005582386</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.76081818851986283</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.78802667122782466</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.79467261081130947</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.80759074765924088</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0.81480430837725581</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.81238622370242686</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0.79351072691234414</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.79300545548775292</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.7409151370622481</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.77487419957513193</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0.79995472124998268</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.7692505209587811</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0.76612223671238655</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0.78926792362212639</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>0.79098576757245864</v>
+      </c>
+      <c r="R8" s="12">
+        <v>0.72908913765680294</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0.72033717479405757</v>
+      </c>
+      <c r="T8" s="12">
+        <v>0.74670155878968303</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0.72151254170744272</v>
+      </c>
+      <c r="V8" s="12">
+        <v>0.65784287477875458</v>
+      </c>
+      <c r="W8" s="12">
+        <v>0.70530840509868675</v>
+      </c>
+      <c r="X8" s="12">
+        <v>0.54796379753989866</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>0.62404250888700497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.4347239518472397</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1.2712743877127439</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1.266085512660855</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1.4217517642175177</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1.2681159420289856</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.4951856263648997</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1.4331447290053603</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1.2480242360379346</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0.7913735653461681</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0.59863557295064151</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0.66634809387278326</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0.80505999787618143</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0.84355421047042589</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0.75727407879367103</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0.69974083672713816</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>0.71331932062525671</v>
+      </c>
+      <c r="R9" s="14">
+        <v>0.68855548307603109</v>
+      </c>
+      <c r="S9" s="14">
+        <v>0.73204319779662241</v>
+      </c>
+      <c r="T9" s="14">
+        <v>0.63781981590200776</v>
+      </c>
+      <c r="U9" s="14">
+        <v>0.64687975646879758</v>
+      </c>
+      <c r="V9" s="14">
+        <v>0.59019441698441844</v>
+      </c>
+      <c r="W9" s="14">
+        <v>0.59195970437320533</v>
+      </c>
+      <c r="X9" s="14">
+        <v>0.61490844042743487</v>
+      </c>
+      <c r="Y9" s="14">
+        <v>0.57136468483735825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="I10" s="12">
+        <v>7.6103500761035017E-2</v>
+      </c>
+      <c r="J10" s="12">
+        <v>5.7077625570776259E-2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>6.9308545335942592E-2</v>
+      </c>
+      <c r="L10" s="12">
+        <v>6.8054092026694768E-2</v>
+      </c>
+      <c r="M10" s="12">
+        <v>8.8660578386605779E-2</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0.11598801893510953</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0.11220942299709424</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0.12097049001567504</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>0.12390801069286163</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0.1283875941410188</v>
+      </c>
+      <c r="S10" s="12">
+        <v>0.1271485317592902</v>
+      </c>
+      <c r="T10" s="12">
+        <v>0.12814312199794212</v>
+      </c>
+      <c r="U10" s="12">
+        <v>0.12935469333265309</v>
+      </c>
+      <c r="V10" s="12">
+        <v>0.12621188286312468</v>
+      </c>
+      <c r="W10" s="12">
+        <v>0.12001537697017431</v>
+      </c>
+      <c r="X10" s="12">
+        <v>0.12915663284776227</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>0.1291537512915375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.14269406392694065</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.21200260926288322</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.22015655577299412</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.20236612702366127</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.18708777270421106</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.15882469724042089</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.17649535282878334</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0.20928462709284626</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.19104217029277468</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0.19715459312875117</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.19199715674230658</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0.20889060009186458</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0.22771047468183536</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0.22565247560211299</v>
+      </c>
+      <c r="P11" s="14">
+        <v>0.21490966845344453</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>0.23739859023806356</v>
+      </c>
+      <c r="R11" s="14">
+        <v>0.21094548568767438</v>
+      </c>
+      <c r="S11" s="14">
+        <v>0.20810079485878574</v>
+      </c>
+      <c r="T11" s="14">
+        <v>0.21911679078177193</v>
+      </c>
+      <c r="U11" s="14">
+        <v>0.24123373826139399</v>
+      </c>
+      <c r="V11" s="14">
+        <v>0.259420086117576</v>
+      </c>
+      <c r="W11" s="14">
+        <v>0.22664894337161073</v>
+      </c>
+      <c r="X11" s="14">
+        <v>0.21152457876108918</v>
+      </c>
+      <c r="Y11" s="14">
+        <v>0.24995886297256162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E16" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H16" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I16" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J16" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K16" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L16" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M16" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N16" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O16" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P16" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R16" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S16" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T16" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U16" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V16" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W16" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X16" s="10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.65507145273127021</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.70855841068035541</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.6572836882190054</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.66795828727795103</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.62441319864710465</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.61153310682623163</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0.57753151026969707</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.59143141855243575</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.57563238385156201</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0.57671093237261395</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0.54659134266267884</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0.48959346018435024</v>
+      </c>
+      <c r="N17" s="12">
+        <v>0.47204644576248633</v>
+      </c>
+      <c r="O17" s="12">
+        <v>0.46064340026918904</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0.46706407389769605</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>0.48648885924182372</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0.51708852636124003</v>
+      </c>
+      <c r="S17" s="12">
+        <v>0.51871573462922282</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0.4969645862171681</v>
+      </c>
+      <c r="U17" s="12">
+        <v>0.49137811601855713</v>
+      </c>
+      <c r="V17" s="12">
+        <v>0.51787948529646377</v>
+      </c>
+      <c r="W17" s="12">
+        <v>0.5341149748927575</v>
+      </c>
+      <c r="X17" s="12">
+        <v>0.54240480484752174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14">
+        <v>0.47682418559038953</v>
+      </c>
+      <c r="N18" s="14">
+        <v>0.47787079316759684</v>
+      </c>
+      <c r="O18" s="14">
+        <v>0.68608066971080672</v>
+      </c>
+      <c r="P18" s="14">
+        <v>0.63251902587519038</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>0.71154709387818282</v>
+      </c>
+      <c r="R18" s="14">
+        <v>0.68991475465456553</v>
+      </c>
+      <c r="S18" s="14">
+        <v>0.94102096498296517</v>
+      </c>
+      <c r="T18" s="14">
+        <v>0.89751473769031775</v>
+      </c>
+      <c r="U18" s="14">
+        <v>0.90819514539774093</v>
+      </c>
+      <c r="V18" s="14">
+        <v>0.94150868710858548</v>
+      </c>
+      <c r="W18" s="14">
+        <v>0.70902073879299388</v>
+      </c>
+      <c r="X18" s="14">
+        <v>0.80293905593960735</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.32282078015860649</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.35595105709784614</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.29729053112042492</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0.29083409798800802</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0.29496174796927549</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0.25589254143295048</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0.28033326413732557</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0.28707591471688315</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0.31068978946717857</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0.28061596014311618</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0.30318205573739576</v>
+      </c>
+      <c r="M19" s="12">
+        <v>0.22657361497385858</v>
+      </c>
+      <c r="N19" s="12">
+        <v>0.28814545753169268</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0.34306621642304425</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0.31112192879741829</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>0.27034926347874866</v>
+      </c>
+      <c r="R19" s="12">
+        <v>0.2926659088325631</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0.24483427383365902</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0.31269804580294608</v>
+      </c>
+      <c r="U19" s="12">
+        <v>0.27171404276150501</v>
+      </c>
+      <c r="V19" s="12">
+        <v>0.29510118752862963</v>
+      </c>
+      <c r="W19" s="12">
+        <v>0.28086313296037818</v>
+      </c>
+      <c r="X19" s="12">
+        <v>0.22444913497305133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.75008977690880807</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0.76077483705554294</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.7879893080553233</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.79463498604871241</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.8075543128788194</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.8148025038364537</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.81238802824322898</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0.79351072691234414</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.79300004186534656</v>
+      </c>
+      <c r="K20" s="14">
+        <v>0.74090790403508877</v>
+      </c>
+      <c r="L20" s="14">
+        <v>0.77487600783192179</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0.79995067617954385</v>
+      </c>
+      <c r="N20" s="14">
+        <v>0.76924331867198725</v>
+      </c>
+      <c r="O20" s="14">
+        <v>0.76613068307985177</v>
+      </c>
+      <c r="P20" s="14">
+        <v>0.78926613163964765</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>0.79098180387357531</v>
+      </c>
+      <c r="R20" s="14">
+        <v>0.72908096795262656</v>
+      </c>
+      <c r="S20" s="14">
+        <v>0.72033559980239359</v>
+      </c>
+      <c r="T20" s="14">
+        <v>0.74670483535098608</v>
+      </c>
+      <c r="U20" s="14">
+        <v>0.72151541141096831</v>
+      </c>
+      <c r="V20" s="14">
+        <v>0.65784820512248465</v>
+      </c>
+      <c r="W20" s="14">
+        <v>0.70531080719289641</v>
+      </c>
+      <c r="X20" s="14">
+        <v>0.54796572739577298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="12">
+        <v>3.6927707854271789E-2</v>
+      </c>
+      <c r="C21" s="12">
+        <v>3.2106164383561647E-2</v>
+      </c>
+      <c r="D21" s="12">
+        <v>3.0674905885911357E-2</v>
+      </c>
+      <c r="E21" s="12">
+        <v>3.723476881607915E-2</v>
+      </c>
+      <c r="F21" s="12">
+        <v>3.5518030365180489E-2</v>
+      </c>
+      <c r="G21" s="12">
+        <v>4.2416457904387937E-2</v>
+      </c>
+      <c r="H21" s="12">
+        <v>3.9887577105863672E-2</v>
+      </c>
+      <c r="I21" s="12">
+        <v>3.815298856026976E-2</v>
+      </c>
+      <c r="J21" s="12">
+        <v>3.4664567786608445E-2</v>
+      </c>
+      <c r="K21" s="12">
+        <v>3.0554855784857463E-2</v>
+      </c>
+      <c r="L21" s="12">
+        <v>3.1924978980746692E-2</v>
+      </c>
+      <c r="M21" s="12">
+        <v>4.2420421651444461E-2</v>
+      </c>
+      <c r="N21" s="12">
+        <v>4.4328624511802063E-2</v>
+      </c>
+      <c r="O21" s="12">
+        <v>4.3455693252832557E-2</v>
+      </c>
+      <c r="P21" s="12">
+        <v>4.654041069231591E-2</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>4.4431352478279694E-2</v>
+      </c>
+      <c r="R21" s="12">
+        <v>4.8236179261924875E-2</v>
+      </c>
+      <c r="S21" s="12">
+        <v>5.73174118940072E-2</v>
+      </c>
+      <c r="T21" s="12">
+        <v>5.2895430041181767E-2</v>
+      </c>
+      <c r="U21" s="12">
+        <v>5.3900035971085496E-2</v>
+      </c>
+      <c r="V21" s="12">
+        <v>5.1096165415330838E-2</v>
+      </c>
+      <c r="W21" s="12">
+        <v>5.0187342643328442E-2</v>
+      </c>
+      <c r="X21" s="12">
+        <v>4.9969373471372251E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="14">
+        <v>8.51761252446184E-2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.10047292889758642</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0.10136986301369863</v>
+      </c>
+      <c r="E22" s="14">
+        <v>9.8515981735159838E-2</v>
+      </c>
+      <c r="F22" s="14">
+        <v>8.7671232876712343E-2</v>
+      </c>
+      <c r="G22" s="14">
+        <v>9.2211099402880234E-2</v>
+      </c>
+      <c r="H22" s="14">
+        <v>9.2108066971080677E-2</v>
+      </c>
+      <c r="I22" s="14">
+        <v>7.7151387425360041E-2</v>
+      </c>
+      <c r="J22" s="14">
+        <v>5.9492009132420094E-2</v>
+      </c>
+      <c r="K22" s="14">
+        <v>7.1695679409195065E-2</v>
+      </c>
+      <c r="L22" s="14">
+        <v>6.7793348379082907E-2</v>
+      </c>
+      <c r="M22" s="14">
+        <v>8.9144951765142907E-2</v>
+      </c>
+      <c r="N22" s="14">
+        <v>0.11753105059980719</v>
+      </c>
+      <c r="O22" s="14">
+        <v>0.11489224215382465</v>
+      </c>
+      <c r="P22" s="14">
+        <v>0.12448158526861221</v>
+      </c>
+      <c r="Q22" s="14">
+        <v>0.12979460687322764</v>
+      </c>
+      <c r="R22" s="14">
+        <v>0.13506891572810997</v>
+      </c>
+      <c r="S22" s="14">
+        <v>0.13509952073241918</v>
+      </c>
+      <c r="T22" s="14">
+        <v>0.13660941729581461</v>
+      </c>
+      <c r="U22" s="14">
+        <v>0.13869028839168057</v>
+      </c>
+      <c r="V22" s="14">
+        <v>0.1352356616976321</v>
+      </c>
+      <c r="W22" s="14">
+        <v>0.13037828662205719</v>
+      </c>
+      <c r="X22" s="14">
+        <v>0.15496417492770403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.14467676039413602</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.22699598726995987</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.21969922572960091</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.20304448912906872</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.18967947246243719</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0.15924988419032496</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.17645394336864709</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0.20900784040654269</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0.19101497872545981</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0.19710765174028208</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0.19202855734949736</v>
+      </c>
+      <c r="M23" s="12">
+        <v>0.20897927349870182</v>
+      </c>
+      <c r="N23" s="12">
+        <v>0.22776141636182795</v>
+      </c>
+      <c r="O23" s="12">
+        <v>0.2257468487267531</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0.21492394513606378</v>
+      </c>
+      <c r="Q23" s="12">
+        <v>0.23744797980775009</v>
+      </c>
+      <c r="R23" s="12">
+        <v>0.21101790768326553</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0.20810602325113201</v>
+      </c>
+      <c r="T23" s="12">
+        <v>0.21910392366842035</v>
+      </c>
+      <c r="U23" s="12">
+        <v>0.24129166336449459</v>
+      </c>
+      <c r="V23" s="12">
+        <v>0.26069700487040792</v>
+      </c>
+      <c r="W23" s="12">
+        <v>0.22841616489062896</v>
+      </c>
+      <c r="X23" s="12">
+        <v>0.20822393273037404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A28" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D28" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F28" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G28" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H28" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I28" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J28" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K28" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L28" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M28" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N28" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O28" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P28" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R28" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S28" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T28" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U28" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V28" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W28" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X28" s="10">
+        <v>2022</v>
+      </c>
+      <c r="Y28" s="10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A29" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.67</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.77</v>
+      </c>
+      <c r="F29" s="15">
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="H29" s="15">
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0.94</v>
+      </c>
+      <c r="J29" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="K29" s="15">
+        <v>1.04</v>
+      </c>
+      <c r="L29" s="16">
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="M29" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="N29" s="16">
+        <v>1.51</v>
+      </c>
+      <c r="O29" s="16">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="P29" s="16">
+        <v>1.7</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>1.77</v>
+      </c>
+      <c r="R29" s="16">
+        <v>1.9</v>
+      </c>
+      <c r="S29" s="16">
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="T29" s="16">
+        <v>2.16</v>
+      </c>
+      <c r="U29" s="16">
+        <v>2.2399999999999998</v>
+      </c>
+      <c r="V29" s="16">
+        <v>2.16</v>
+      </c>
+      <c r="W29" s="16">
+        <v>2.27</v>
+      </c>
+      <c r="X29" s="16">
+        <v>2.29</v>
+      </c>
+      <c r="Y29" s="16">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A30" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="17">
+        <v>8.4</v>
+      </c>
+      <c r="C30" s="17">
+        <v>8.4</v>
+      </c>
+      <c r="D30" s="17">
+        <v>8.4</v>
+      </c>
+      <c r="E30" s="17">
+        <v>8.4</v>
+      </c>
+      <c r="F30" s="17">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="G30" s="17">
+        <v>7.72</v>
+      </c>
+      <c r="H30" s="17">
+        <v>7.53</v>
+      </c>
+      <c r="I30" s="17">
+        <v>7.53</v>
+      </c>
+      <c r="J30" s="17">
+        <v>7.63</v>
+      </c>
+      <c r="K30" s="17">
+        <v>7.63</v>
+      </c>
+      <c r="L30" s="18">
+        <v>7.63</v>
+      </c>
+      <c r="M30" s="18">
+        <v>7.63</v>
+      </c>
+      <c r="N30" s="18">
+        <v>7.9</v>
+      </c>
+      <c r="O30" s="18">
+        <v>6.31</v>
+      </c>
+      <c r="P30" s="18">
+        <v>5.8</v>
+      </c>
+      <c r="Q30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="R30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="S30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="T30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="U30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="V30" s="18">
+        <v>3.74</v>
+      </c>
+      <c r="W30" s="18">
+        <v>3.11</v>
+      </c>
+      <c r="X30" s="18">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="Y30" s="18">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="15">
+        <v>25.27</v>
+      </c>
+      <c r="C31" s="15">
+        <v>26.17</v>
+      </c>
+      <c r="D31" s="15">
+        <v>26.91</v>
+      </c>
+      <c r="E31" s="15">
+        <v>26.51</v>
+      </c>
+      <c r="F31" s="15">
+        <v>26.17</v>
+      </c>
+      <c r="G31" s="15">
+        <v>25.45</v>
+      </c>
+      <c r="H31" s="15">
+        <v>24.64</v>
+      </c>
+      <c r="I31" s="15">
+        <v>24.37</v>
+      </c>
+      <c r="J31" s="15">
+        <v>24.23</v>
+      </c>
+      <c r="K31" s="15">
+        <v>25.82</v>
+      </c>
+      <c r="L31" s="16">
+        <v>27.02</v>
+      </c>
+      <c r="M31" s="16">
+        <v>26.74</v>
+      </c>
+      <c r="N31" s="16">
+        <v>27.69</v>
+      </c>
+      <c r="O31" s="16">
+        <v>25.52</v>
+      </c>
+      <c r="P31" s="16">
+        <v>23.75</v>
+      </c>
+      <c r="Q31" s="16">
+        <v>23.66</v>
+      </c>
+      <c r="R31" s="16">
+        <v>22.55</v>
+      </c>
+      <c r="S31" s="16">
+        <v>19.52</v>
+      </c>
+      <c r="T31" s="16">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="U31" s="16">
+        <v>17.11</v>
+      </c>
+      <c r="V31" s="16">
+        <v>17.39</v>
+      </c>
+      <c r="W31" s="16">
+        <v>17.25</v>
+      </c>
+      <c r="X31" s="16">
+        <v>17.79</v>
+      </c>
+      <c r="Y31" s="16">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A32" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="17">
+        <v>23.3</v>
+      </c>
+      <c r="C32" s="17">
+        <v>23.32</v>
+      </c>
+      <c r="D32" s="17">
+        <v>23.42</v>
+      </c>
+      <c r="E32" s="17">
+        <v>23.43</v>
+      </c>
+      <c r="F32" s="17">
+        <v>23.32</v>
+      </c>
+      <c r="G32" s="17">
+        <v>23.33</v>
+      </c>
+      <c r="H32" s="17">
+        <v>23.34</v>
+      </c>
+      <c r="I32" s="17">
+        <v>23.35</v>
+      </c>
+      <c r="J32" s="17">
+        <v>23.31</v>
+      </c>
+      <c r="K32" s="17">
+        <v>23.4</v>
+      </c>
+      <c r="L32" s="18">
+        <v>23.62</v>
+      </c>
+      <c r="M32" s="18">
+        <v>23.83</v>
+      </c>
+      <c r="N32" s="18">
+        <v>23.85</v>
+      </c>
+      <c r="O32" s="18">
+        <v>23.84</v>
+      </c>
+      <c r="P32" s="18">
+        <v>23.8</v>
+      </c>
+      <c r="Q32" s="18">
+        <v>23.82</v>
+      </c>
+      <c r="R32" s="18">
+        <v>23.89</v>
+      </c>
+      <c r="S32" s="18">
+        <v>23.98</v>
+      </c>
+      <c r="T32" s="18">
+        <v>24</v>
+      </c>
+      <c r="U32" s="18">
+        <v>24.14</v>
+      </c>
+      <c r="V32" s="18">
+        <v>24.23</v>
+      </c>
+      <c r="W32" s="18">
+        <v>24.26</v>
+      </c>
+      <c r="X32" s="18">
+        <v>24.24</v>
+      </c>
+      <c r="Y32" s="18">
+        <v>24.14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="15">
+        <v>63.18</v>
+      </c>
+      <c r="C33" s="15">
+        <v>63.18</v>
+      </c>
+      <c r="D33" s="15">
+        <v>63.27</v>
+      </c>
+      <c r="E33" s="15">
+        <v>63.36</v>
+      </c>
+      <c r="F33" s="15">
+        <v>63.36</v>
+      </c>
+      <c r="G33" s="15">
+        <v>63.26</v>
+      </c>
+      <c r="H33" s="15">
+        <v>63.26</v>
+      </c>
+      <c r="I33" s="15">
+        <v>63.26</v>
+      </c>
+      <c r="J33" s="15">
+        <v>63.26</v>
+      </c>
+      <c r="K33" s="15">
+        <v>63.13</v>
+      </c>
+      <c r="L33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="M33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="N33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="O33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="P33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="Q33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="R33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="S33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="T33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="U33" s="16">
+        <v>63.13</v>
+      </c>
+      <c r="V33" s="16">
+        <v>61.4</v>
+      </c>
+      <c r="W33" s="16">
+        <v>61.4</v>
+      </c>
+      <c r="X33" s="16">
+        <v>61.4</v>
+      </c>
+      <c r="Y33" s="16">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="C34" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="E34" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="H34" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="I34" s="17">
+        <v>1.04</v>
+      </c>
+      <c r="J34" s="17">
+        <v>1.48</v>
+      </c>
+      <c r="K34" s="17">
+        <v>1.68</v>
+      </c>
+      <c r="L34" s="18">
+        <v>1.72</v>
+      </c>
+      <c r="M34" s="18">
+        <v>1.72</v>
+      </c>
+      <c r="N34" s="18">
+        <v>1.72</v>
+      </c>
+      <c r="O34" s="18">
+        <v>1.72</v>
+      </c>
+      <c r="P34" s="18">
+        <v>1.85</v>
+      </c>
+      <c r="Q34" s="18">
+        <v>1.89</v>
+      </c>
+      <c r="R34" s="18">
+        <v>1.89</v>
+      </c>
+      <c r="S34" s="18">
+        <v>1.89</v>
+      </c>
+      <c r="T34" s="18">
+        <v>1.89</v>
+      </c>
+      <c r="U34" s="18">
+        <v>1.89</v>
+      </c>
+      <c r="V34" s="18">
+        <v>1.94</v>
+      </c>
+      <c r="W34" s="18">
+        <v>1.94</v>
+      </c>
+      <c r="X34" s="18">
+        <v>1.94</v>
+      </c>
+      <c r="Y34" s="18">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A35" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="J35" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="K35" s="15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L35" s="16">
+        <v>1.04</v>
+      </c>
+      <c r="M35" s="16">
+        <v>3</v>
+      </c>
+      <c r="N35" s="16">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="O35" s="16">
+        <v>5.28</v>
+      </c>
+      <c r="P35" s="16">
+        <v>6.03</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>7.14</v>
+      </c>
+      <c r="R35" s="16">
+        <v>7.7</v>
+      </c>
+      <c r="S35" s="16">
+        <v>8.61</v>
+      </c>
+      <c r="T35" s="16">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="U35" s="16">
+        <v>10.74</v>
+      </c>
+      <c r="V35" s="16">
+        <v>11.93</v>
+      </c>
+      <c r="W35" s="16">
+        <v>14.61</v>
+      </c>
+      <c r="X35" s="16">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="Y35" s="16">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A36" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="C36" s="17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D36" s="17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E36" s="17">
+        <v>0.22</v>
+      </c>
+      <c r="F36" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0.69</v>
+      </c>
+      <c r="H36" s="17">
+        <v>1.41</v>
+      </c>
+      <c r="I36" s="17">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="J36" s="17">
+        <v>3.4</v>
+      </c>
+      <c r="K36" s="17">
+        <v>4.58</v>
+      </c>
+      <c r="L36" s="18">
+        <v>5.91</v>
+      </c>
+      <c r="M36" s="18">
+        <v>6.76</v>
+      </c>
+      <c r="N36" s="18">
+        <v>7.61</v>
+      </c>
+      <c r="O36" s="18">
+        <v>8.16</v>
+      </c>
+      <c r="P36" s="18">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>10.3</v>
+      </c>
+      <c r="R36" s="18">
+        <v>11.57</v>
+      </c>
+      <c r="S36" s="18">
+        <v>13.5</v>
+      </c>
+      <c r="T36" s="18">
+        <v>14.9</v>
+      </c>
+      <c r="U36" s="18">
+        <v>16.43</v>
+      </c>
+      <c r="V36" s="18">
+        <v>17.54</v>
+      </c>
+      <c r="W36" s="18">
+        <v>18.55</v>
+      </c>
+      <c r="X36" s="18">
+        <v>20.81</v>
+      </c>
+      <c r="Y36" s="18">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A41" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C41" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D41" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E41" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F41" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G41" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H41" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I41" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J41" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K41" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L41" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M41" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N41" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O41" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P41" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q41" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R41" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S41" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T41" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U41" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V41" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W41" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X41" s="10">
+        <v>2022</v>
+      </c>
+      <c r="Y41" s="10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A42" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="16">
+        <v>2.99</v>
+      </c>
+      <c r="C42" s="16">
+        <v>3.33</v>
+      </c>
+      <c r="D42" s="16">
+        <v>3.5300000000000002</v>
+      </c>
+      <c r="E42" s="16">
+        <v>3.7199999999999998</v>
+      </c>
+      <c r="F42" s="16">
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="G42" s="16">
+        <v>3.87</v>
+      </c>
+      <c r="H42" s="16">
+        <v>3.84</v>
+      </c>
+      <c r="I42" s="16">
+        <v>4.22</v>
+      </c>
+      <c r="J42" s="16">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="K42" s="16">
+        <v>4.58</v>
+      </c>
+      <c r="L42" s="16">
+        <v>4.92</v>
+      </c>
+      <c r="M42" s="16">
+        <v>5.58</v>
+      </c>
+      <c r="N42" s="16">
+        <v>5.81</v>
+      </c>
+      <c r="O42" s="16">
+        <v>6.18</v>
+      </c>
+      <c r="P42" s="16">
+        <v>6.5500000000000007</v>
+      </c>
+      <c r="Q42" s="16">
+        <v>7.11</v>
+      </c>
+      <c r="R42" s="16">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="S42" s="16">
+        <v>8.43</v>
+      </c>
+      <c r="T42" s="16">
+        <v>8.99</v>
+      </c>
+      <c r="U42" s="16">
+        <v>9.25</v>
+      </c>
+      <c r="V42" s="16">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="W42" s="16">
+        <v>10.15</v>
+      </c>
+      <c r="X42" s="16">
+        <v>10.379999999999999</v>
+      </c>
+      <c r="Y42" s="16">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A43" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="18">
+        <v>27</v>
+      </c>
+      <c r="C43" s="18">
+        <v>20.48</v>
+      </c>
+      <c r="D43" s="18">
+        <v>23.66</v>
+      </c>
+      <c r="E43" s="18">
+        <v>26.26</v>
+      </c>
+      <c r="F43" s="18">
+        <v>24.37</v>
+      </c>
+      <c r="G43" s="18">
+        <v>27.51</v>
+      </c>
+      <c r="H43" s="18">
+        <v>22.89</v>
+      </c>
+      <c r="I43" s="18">
+        <v>24.45</v>
+      </c>
+      <c r="J43" s="18">
+        <v>23.06</v>
+      </c>
+      <c r="K43" s="18">
+        <v>21.67</v>
+      </c>
+      <c r="L43" s="18">
+        <v>23.36</v>
+      </c>
+      <c r="M43" s="18">
+        <v>17.39</v>
+      </c>
+      <c r="N43" s="18">
+        <v>21.46</v>
+      </c>
+      <c r="O43" s="18">
+        <v>23.84</v>
+      </c>
+      <c r="P43" s="18">
+        <v>11.26</v>
+      </c>
+      <c r="Q43" s="18">
+        <v>11.89</v>
+      </c>
+      <c r="R43" s="18">
+        <v>10.23</v>
+      </c>
+      <c r="S43" s="18">
+        <v>12.81</v>
+      </c>
+      <c r="T43" s="18">
+        <v>8.31</v>
+      </c>
+      <c r="U43" s="18">
+        <v>3.64</v>
+      </c>
+      <c r="V43" s="18">
+        <v>3.09</v>
+      </c>
+      <c r="W43" s="18">
+        <v>5.44</v>
+      </c>
+      <c r="X43" s="18">
+        <v>4.33</v>
+      </c>
+      <c r="Y43" s="18">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="16">
+        <v>11.51</v>
+      </c>
+      <c r="C44" s="16">
+        <v>15.15</v>
+      </c>
+      <c r="D44" s="16">
+        <v>18.37</v>
+      </c>
+      <c r="E44" s="16">
+        <v>19.37</v>
+      </c>
+      <c r="F44" s="16">
+        <v>21.05</v>
+      </c>
+      <c r="G44" s="16">
+        <v>23.07</v>
+      </c>
+      <c r="H44" s="16">
+        <v>21.76</v>
+      </c>
+      <c r="I44" s="16">
+        <v>21.99</v>
+      </c>
+      <c r="J44" s="16">
+        <v>21.88</v>
+      </c>
+      <c r="K44" s="16">
+        <v>20.5</v>
+      </c>
+      <c r="L44" s="16">
+        <v>23.76</v>
+      </c>
+      <c r="M44" s="16">
+        <v>29.49</v>
+      </c>
+      <c r="N44" s="16">
+        <v>22.75</v>
+      </c>
+      <c r="O44" s="16">
+        <v>18.39</v>
+      </c>
+      <c r="P44" s="16">
+        <v>13.16</v>
+      </c>
+      <c r="Q44" s="16">
+        <v>21.14</v>
+      </c>
+      <c r="R44" s="16">
+        <v>34.97</v>
+      </c>
+      <c r="S44" s="16">
+        <v>40.5</v>
+      </c>
+      <c r="T44" s="16">
+        <v>30.61</v>
+      </c>
+      <c r="U44" s="16">
+        <v>39.31</v>
+      </c>
+      <c r="V44" s="16">
+        <v>35.25</v>
+      </c>
+      <c r="W44" s="16">
+        <v>33.29</v>
+      </c>
+      <c r="X44" s="16">
+        <v>45.74</v>
+      </c>
+      <c r="Y44" s="16">
+        <v>31.43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A45" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="18">
+        <v>64.78</v>
+      </c>
+      <c r="C45" s="18">
+        <v>72.62</v>
+      </c>
+      <c r="D45" s="18">
+        <v>58.88</v>
+      </c>
+      <c r="E45" s="18">
+        <v>57.35</v>
+      </c>
+      <c r="F45" s="18">
+        <v>58.04</v>
+      </c>
+      <c r="G45" s="18">
+        <v>50.14</v>
+      </c>
+      <c r="H45" s="18">
+        <v>54.88</v>
+      </c>
+      <c r="I45" s="18">
+        <v>55.99</v>
+      </c>
+      <c r="J45" s="18">
+        <v>62.16</v>
+      </c>
+      <c r="K45" s="18">
+        <v>55.49</v>
+      </c>
+      <c r="L45" s="18">
+        <v>61.2</v>
+      </c>
+      <c r="M45" s="18">
+        <v>45.74</v>
+      </c>
+      <c r="N45" s="18">
+        <v>59.83</v>
+      </c>
+      <c r="O45" s="18">
+        <v>71.92</v>
+      </c>
+      <c r="P45" s="18">
+        <v>63.77</v>
+      </c>
+      <c r="Q45" s="18">
+        <v>55.56</v>
+      </c>
+      <c r="R45" s="18">
+        <v>60.84</v>
+      </c>
+      <c r="S45" s="18">
+        <v>50</v>
+      </c>
+      <c r="T45" s="18">
+        <v>65.11</v>
+      </c>
+      <c r="U45" s="18">
+        <v>56.91</v>
+      </c>
+      <c r="V45" s="18">
+        <v>62.59</v>
+      </c>
+      <c r="W45" s="18">
+        <v>59.62</v>
+      </c>
+      <c r="X45" s="18">
+        <v>45.52</v>
+      </c>
+      <c r="Y45" s="18">
+        <v>53.19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A46" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="16">
+        <v>415.16</v>
+      </c>
+      <c r="C46" s="16">
+        <v>421.08</v>
+      </c>
+      <c r="D46" s="16">
+        <v>436.76</v>
+      </c>
+      <c r="E46" s="16">
+        <v>441.07</v>
+      </c>
+      <c r="F46" s="16">
+        <v>448.24</v>
+      </c>
+      <c r="G46" s="16">
+        <v>451.53</v>
+      </c>
+      <c r="H46" s="16">
+        <v>450.19</v>
+      </c>
+      <c r="I46" s="16">
+        <v>439.73</v>
+      </c>
+      <c r="J46" s="16">
+        <v>439.45</v>
+      </c>
+      <c r="K46" s="16">
+        <v>409.74</v>
+      </c>
+      <c r="L46" s="16">
+        <v>428.52</v>
+      </c>
+      <c r="M46" s="16">
+        <v>442.39</v>
+      </c>
+      <c r="N46" s="16">
+        <v>425.41</v>
+      </c>
+      <c r="O46" s="16">
+        <v>423.68</v>
+      </c>
+      <c r="P46" s="16">
+        <v>436.48</v>
+      </c>
+      <c r="Q46" s="16">
+        <v>437.43</v>
+      </c>
+      <c r="R46" s="16">
+        <v>403.2</v>
+      </c>
+      <c r="S46" s="16">
+        <v>398.36</v>
+      </c>
+      <c r="T46" s="16">
+        <v>412.94</v>
+      </c>
+      <c r="U46" s="16">
+        <v>399.01</v>
+      </c>
+      <c r="V46" s="16">
+        <v>353.83</v>
+      </c>
+      <c r="W46" s="16">
+        <v>379.36</v>
+      </c>
+      <c r="X46" s="16">
+        <v>294.73</v>
+      </c>
+      <c r="Y46" s="16">
+        <v>335.65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A47" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="18">
+        <v>11.06</v>
+      </c>
+      <c r="C47" s="18">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D47" s="18">
+        <v>9.76</v>
+      </c>
+      <c r="E47" s="18">
+        <v>10.96</v>
+      </c>
+      <c r="F47" s="18">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="G47" s="18">
+        <v>12.05</v>
+      </c>
+      <c r="H47" s="18">
+        <v>11.55</v>
+      </c>
+      <c r="I47" s="18">
+        <v>11.37</v>
+      </c>
+      <c r="J47" s="18">
+        <v>10.26</v>
+      </c>
+      <c r="K47" s="18">
+        <v>8.81</v>
+      </c>
+      <c r="L47" s="18">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="M47" s="18">
+        <v>12.13</v>
+      </c>
+      <c r="N47" s="18">
+        <v>12.71</v>
+      </c>
+      <c r="O47" s="18">
+        <v>11.41</v>
+      </c>
+      <c r="P47" s="18">
+        <v>11.34</v>
+      </c>
+      <c r="Q47" s="18">
+        <v>11.81</v>
+      </c>
+      <c r="R47" s="18">
+        <v>11.4</v>
+      </c>
+      <c r="S47" s="18">
+        <v>12.12</v>
+      </c>
+      <c r="T47" s="18">
+        <v>10.56</v>
+      </c>
+      <c r="U47" s="18">
+        <v>10.71</v>
+      </c>
+      <c r="V47" s="18">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="W47" s="18">
+        <v>10.06</v>
+      </c>
+      <c r="X47" s="18">
+        <v>10.45</v>
+      </c>
+      <c r="Y47" s="18">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="D48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="E48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="G48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="H48" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="I48" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="J48" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="K48" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="L48" s="16">
+        <v>0.62</v>
+      </c>
+      <c r="M48" s="16">
+        <v>2.33</v>
+      </c>
+      <c r="N48" s="16">
+        <v>4.43</v>
+      </c>
+      <c r="O48" s="16">
+        <v>5.19</v>
+      </c>
+      <c r="P48" s="16">
+        <v>6.39</v>
+      </c>
+      <c r="Q48" s="16">
+        <v>7.75</v>
+      </c>
+      <c r="R48" s="16">
+        <v>8.66</v>
+      </c>
+      <c r="S48" s="16">
+        <v>9.59</v>
+      </c>
+      <c r="T48" s="16">
+        <v>10.81</v>
+      </c>
+      <c r="U48" s="16">
+        <v>12.17</v>
+      </c>
+      <c r="V48" s="16">
+        <v>13.19</v>
+      </c>
+      <c r="W48" s="16">
+        <v>15.36</v>
+      </c>
+      <c r="X48" s="16">
+        <v>19.63</v>
+      </c>
+      <c r="Y48" s="16">
+        <v>23.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A49" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="C49" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="D49" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="E49" s="18">
+        <v>0.39</v>
+      </c>
+      <c r="F49" s="18">
+        <v>0.59</v>
+      </c>
+      <c r="G49" s="18">
+        <v>0.96</v>
+      </c>
+      <c r="H49" s="18">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="I49" s="18">
+        <v>4.07</v>
+      </c>
+      <c r="J49" s="18">
+        <v>5.69</v>
+      </c>
+      <c r="K49" s="18">
+        <v>7.91</v>
+      </c>
+      <c r="L49" s="18">
+        <v>9.94</v>
+      </c>
+      <c r="M49" s="18">
+        <v>12.37</v>
+      </c>
+      <c r="N49" s="18">
+        <v>15.18</v>
+      </c>
+      <c r="O49" s="18">
+        <v>16.13</v>
+      </c>
+      <c r="P49" s="18">
+        <v>17.32</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>21.42</v>
+      </c>
+      <c r="R49" s="18">
+        <v>21.38</v>
+      </c>
+      <c r="S49" s="18">
+        <v>24.61</v>
+      </c>
+      <c r="T49" s="18">
+        <v>28.6</v>
+      </c>
+      <c r="U49" s="18">
+        <v>34.72</v>
+      </c>
+      <c r="V49" s="18">
+        <v>39.86</v>
+      </c>
+      <c r="W49" s="18">
+        <v>36.83</v>
+      </c>
+      <c r="X49" s="18">
+        <v>38.56</v>
+      </c>
+      <c r="Y49" s="18">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A54" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C54" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D54" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E54" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F54" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G54" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H54" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I54" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J54" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K54" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L54" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M54" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N54" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O54" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P54" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q54" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R54" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S54" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T54" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U54" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V54" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W54" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X54" s="10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A55" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="16">
+        <v>2.4790000000000001</v>
+      </c>
+      <c r="C55" s="16">
+        <v>2.8490000000000002</v>
+      </c>
+      <c r="D55" s="16">
+        <v>3.0430000000000001</v>
+      </c>
+      <c r="E55" s="16">
+        <v>3.2269999999999999</v>
+      </c>
+      <c r="F55" s="16">
+        <v>3.3119999999999998</v>
+      </c>
+      <c r="G55" s="16">
+        <v>3.391</v>
+      </c>
+      <c r="H55" s="16">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="I55" s="16">
+        <v>3.7509999999999999</v>
+      </c>
+      <c r="J55" s="16">
+        <v>3.9710000000000001</v>
+      </c>
+      <c r="K55" s="16">
+        <v>4.13</v>
+      </c>
+      <c r="L55" s="16">
+        <v>4.4409999999999998</v>
+      </c>
+      <c r="M55" s="16">
+        <v>5.0391110000000001</v>
+      </c>
+      <c r="N55" s="16">
+        <v>5.2972960000000002</v>
+      </c>
+      <c r="O55" s="16">
+        <v>5.6814349999999996</v>
+      </c>
+      <c r="P55" s="16">
+        <v>5.986905000000001</v>
+      </c>
+      <c r="Q55" s="16">
+        <v>6.5257550000000002</v>
+      </c>
+      <c r="R55" s="16">
+        <v>7.5223430000000002</v>
+      </c>
+      <c r="S55" s="16">
+        <v>7.7812460000000003</v>
+      </c>
+      <c r="T55" s="16">
+        <v>8.3781850000000002</v>
+      </c>
+      <c r="U55" s="16">
+        <v>8.6440820000000009</v>
+      </c>
+      <c r="V55" s="16">
+        <v>8.763751000000001</v>
+      </c>
+      <c r="W55" s="16">
+        <v>9.5745869999999993</v>
+      </c>
+      <c r="X55" s="16">
+        <v>9.7810640000000006</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A56" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="18">
+        <v>30.86</v>
+      </c>
+      <c r="C56" s="18">
+        <v>23.901</v>
+      </c>
+      <c r="D56" s="18">
+        <v>26.991</v>
+      </c>
+      <c r="E56" s="18">
+        <v>29.265999999999998</v>
+      </c>
+      <c r="F56" s="18">
+        <v>27.234999999999999</v>
+      </c>
+      <c r="G56" s="18">
+        <v>30.704999999999998</v>
+      </c>
+      <c r="H56" s="18">
+        <v>26.404</v>
+      </c>
+      <c r="I56" s="18">
+        <v>28.196999999999999</v>
+      </c>
+      <c r="J56" s="18">
+        <v>26.434000000000001</v>
+      </c>
+      <c r="K56" s="18">
+        <v>24.018999999999998</v>
+      </c>
+      <c r="L56" s="18">
+        <v>26.315000000000001</v>
+      </c>
+      <c r="M56" s="18">
+        <v>19.877068999999999</v>
+      </c>
+      <c r="N56" s="18">
+        <v>24.130562999999999</v>
+      </c>
+      <c r="O56" s="18">
+        <v>26.343620999999999</v>
+      </c>
+      <c r="P56" s="18">
+        <v>13.832678</v>
+      </c>
+      <c r="Q56" s="18">
+        <v>14.556545</v>
+      </c>
+      <c r="R56" s="18">
+        <v>12.246047000000001</v>
+      </c>
+      <c r="S56" s="18">
+        <v>15.198416</v>
+      </c>
+      <c r="T56" s="18">
+        <v>10.542506999999999</v>
+      </c>
+      <c r="U56" s="18">
+        <v>5.8727089999999995</v>
+      </c>
+      <c r="V56" s="18">
+        <v>4.9435409999999997</v>
+      </c>
+      <c r="W56" s="18">
+        <v>7.3391339999999996</v>
+      </c>
+      <c r="X56" s="18">
+        <v>6.042878</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="16">
+        <v>11.513999999999999</v>
+      </c>
+      <c r="C57" s="16">
+        <v>15.146000000000001</v>
+      </c>
+      <c r="D57" s="16">
+        <v>18.369</v>
+      </c>
+      <c r="E57" s="16">
+        <v>19.367999999999999</v>
+      </c>
+      <c r="F57" s="16">
+        <v>21.048999999999999</v>
+      </c>
+      <c r="G57" s="16">
+        <v>23.068999999999999</v>
+      </c>
+      <c r="H57" s="16">
+        <v>21.76</v>
+      </c>
+      <c r="I57" s="16">
+        <v>21.986999999999998</v>
+      </c>
+      <c r="J57" s="16">
+        <v>21.884</v>
+      </c>
+      <c r="K57" s="16">
+        <v>20.503</v>
+      </c>
+      <c r="L57" s="16">
+        <v>23.757999999999999</v>
+      </c>
+      <c r="M57" s="16">
+        <v>29.489144</v>
+      </c>
+      <c r="N57" s="16">
+        <v>22.753254000000002</v>
+      </c>
+      <c r="O57" s="16">
+        <v>18.393269</v>
+      </c>
+      <c r="P57" s="16">
+        <v>13.162876000000001</v>
+      </c>
+      <c r="Q57" s="16">
+        <v>21.143152999999998</v>
+      </c>
+      <c r="R57" s="16">
+        <v>34.967086000000002</v>
+      </c>
+      <c r="S57" s="16">
+        <v>40.500366</v>
+      </c>
+      <c r="T57" s="16">
+        <v>30.611537000000002</v>
+      </c>
+      <c r="U57" s="16">
+        <v>39.313589</v>
+      </c>
+      <c r="V57" s="16">
+        <v>35.245131999999998</v>
+      </c>
+      <c r="W57" s="16">
+        <v>33.286339999999996</v>
+      </c>
+      <c r="X57" s="16">
+        <v>45.740707</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A58" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18">
+        <v>6.2237000000000001E-2</v>
+      </c>
+      <c r="N58" s="18">
+        <v>5.6513000000000001E-2</v>
+      </c>
+      <c r="O58" s="18">
+        <v>9.0150999999999995E-2</v>
+      </c>
+      <c r="P58" s="18">
+        <v>8.3113000000000006E-2</v>
+      </c>
+      <c r="Q58" s="18">
+        <v>9.1938999999999993E-2</v>
+      </c>
+      <c r="R58" s="18">
+        <v>9.7604999999999997E-2</v>
+      </c>
+      <c r="S58" s="18">
+        <v>0.13313</v>
+      </c>
+      <c r="T58" s="18">
+        <v>0.126975</v>
+      </c>
+      <c r="U58" s="18">
+        <v>0.12848599999999999</v>
+      </c>
+      <c r="V58" s="18">
+        <v>0.13319900000000001</v>
+      </c>
+      <c r="W58" s="18">
+        <v>0.10030800000000001</v>
+      </c>
+      <c r="X58" s="18">
+        <v>0.113595</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A59" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="16">
+        <v>71.133248999999992</v>
+      </c>
+      <c r="C59" s="16">
+        <v>78.511426999999998</v>
+      </c>
+      <c r="D59" s="16">
+        <v>65.830612000000002</v>
+      </c>
+      <c r="E59" s="16">
+        <v>64.278639999999996</v>
+      </c>
+      <c r="F59" s="16">
+        <v>64.898935000000009</v>
+      </c>
+      <c r="G59" s="16">
+        <v>56.331876999999999</v>
+      </c>
+      <c r="H59" s="16">
+        <v>61.741697000000002</v>
+      </c>
+      <c r="I59" s="16">
+        <v>63.259416999999992</v>
+      </c>
+      <c r="J59" s="16">
+        <v>68.367660999999998</v>
+      </c>
+      <c r="K59" s="16">
+        <v>61.966200000000008</v>
+      </c>
+      <c r="L59" s="16">
+        <v>67.525616999999997</v>
+      </c>
+      <c r="M59" s="16">
+        <v>50.893014000000001</v>
+      </c>
+      <c r="N59" s="16">
+        <v>64.759506000000002</v>
+      </c>
+      <c r="O59" s="16">
+        <v>77.070960999999997</v>
+      </c>
+      <c r="P59" s="16">
+        <v>69.570008000000001</v>
+      </c>
+      <c r="Q59" s="16">
+        <v>60.513362999999998</v>
+      </c>
+      <c r="R59" s="16">
+        <v>65.685547999999997</v>
+      </c>
+      <c r="S59" s="16">
+        <v>55.134909999999998</v>
+      </c>
+      <c r="T59" s="16">
+        <v>70.472115000000002</v>
+      </c>
+      <c r="U59" s="16">
+        <v>61.572316000000001</v>
+      </c>
+      <c r="V59" s="16">
+        <v>67.094319999999996</v>
+      </c>
+      <c r="W59" s="16">
+        <v>63.946742000000008</v>
+      </c>
+      <c r="X59" s="16">
+        <v>51.049095999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A60" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="18">
+        <v>415.16199999999998</v>
+      </c>
+      <c r="C60" s="18">
+        <v>421.07600000000002</v>
+      </c>
+      <c r="D60" s="18">
+        <v>436.76</v>
+      </c>
+      <c r="E60" s="18">
+        <v>441.07</v>
+      </c>
+      <c r="F60" s="18">
+        <v>448.24099999999999</v>
+      </c>
+      <c r="G60" s="18">
+        <v>451.529</v>
+      </c>
+      <c r="H60" s="18">
+        <v>450.19099999999997</v>
+      </c>
+      <c r="I60" s="18">
+        <v>439.73</v>
+      </c>
+      <c r="J60" s="18">
+        <v>439.447</v>
+      </c>
+      <c r="K60" s="18">
+        <v>409.73599999999999</v>
+      </c>
+      <c r="L60" s="18">
+        <v>428.52100000000002</v>
+      </c>
+      <c r="M60" s="18">
+        <v>442.38776299999995</v>
+      </c>
+      <c r="N60" s="18">
+        <v>425.40601700000002</v>
+      </c>
+      <c r="O60" s="18">
+        <v>423.68467099999998</v>
+      </c>
+      <c r="P60" s="18">
+        <v>436.47900900000002</v>
+      </c>
+      <c r="Q60" s="18">
+        <v>437.42780800000003</v>
+      </c>
+      <c r="R60" s="18">
+        <v>403.19548200000003</v>
+      </c>
+      <c r="S60" s="18">
+        <v>398.359129</v>
+      </c>
+      <c r="T60" s="18">
+        <v>412.94181199999997</v>
+      </c>
+      <c r="U60" s="18">
+        <v>399.01158700000002</v>
+      </c>
+      <c r="V60" s="18">
+        <v>353.83286700000002</v>
+      </c>
+      <c r="W60" s="18">
+        <v>379.36129199999999</v>
+      </c>
+      <c r="X60" s="18">
+        <v>294.73103800000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A61" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="16">
+        <v>8.2460000000000004</v>
+      </c>
+      <c r="C61" s="16">
+        <v>7.4249999999999998</v>
+      </c>
+      <c r="D61" s="16">
+        <v>7.3040000000000003</v>
+      </c>
+      <c r="E61" s="16">
+        <v>8.7430000000000003</v>
+      </c>
+      <c r="F61" s="16">
+        <v>8.2449999999999992</v>
+      </c>
+      <c r="G61" s="16">
+        <v>9.5820000000000007</v>
+      </c>
+      <c r="H61" s="16">
+        <v>8.7379999999999995</v>
+      </c>
+      <c r="I61" s="16">
+        <v>8.2910000000000004</v>
+      </c>
+      <c r="J61" s="16">
+        <v>7.5021120000000003</v>
+      </c>
+      <c r="K61" s="16">
+        <v>7.0371969999999999</v>
+      </c>
+      <c r="L61" s="16">
+        <v>7.6861130000000006</v>
+      </c>
+      <c r="M61" s="16">
+        <v>10.192698</v>
+      </c>
+      <c r="N61" s="16">
+        <v>10.320116000000001</v>
+      </c>
+      <c r="O61" s="16">
+        <v>9.3096980000000009</v>
+      </c>
+      <c r="P61" s="16">
+        <v>9.2767210000000002</v>
+      </c>
+      <c r="Q61" s="16">
+        <v>9.5215200000000006</v>
+      </c>
+      <c r="R61" s="16">
+        <v>9.8005120000000012</v>
+      </c>
+      <c r="S61" s="16">
+        <v>10.117649999999999</v>
+      </c>
+      <c r="T61" s="16">
+        <v>8.7252700000000001</v>
+      </c>
+      <c r="U61" s="16">
+        <v>8.8661490000000018</v>
+      </c>
+      <c r="V61" s="16">
+        <v>8.525974999999999</v>
+      </c>
+      <c r="W61" s="16">
+        <v>8.5136489999999991</v>
+      </c>
+      <c r="X61" s="16">
+        <v>9.1636629999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A62" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="18">
+        <v>5.2230000000000002E-3</v>
+      </c>
+      <c r="C62" s="18">
+        <v>6.1609999999999998E-3</v>
+      </c>
+      <c r="D62" s="18">
+        <v>7.1040000000000001E-3</v>
+      </c>
+      <c r="E62" s="18">
+        <v>7.7670000000000005E-3</v>
+      </c>
+      <c r="F62" s="18">
+        <v>8.4480000000000006E-3</v>
+      </c>
+      <c r="G62" s="18">
+        <v>1.0501E-2</v>
+      </c>
+      <c r="H62" s="18">
+        <v>1.2102999999999999E-2</v>
+      </c>
+      <c r="I62" s="18">
+        <v>1.7572000000000001E-2</v>
+      </c>
+      <c r="J62" s="18">
+        <v>4.1692E-2</v>
+      </c>
+      <c r="K62" s="18">
+        <v>0.17397100000000001</v>
+      </c>
+      <c r="L62" s="18">
+        <v>0.62</v>
+      </c>
+      <c r="M62" s="18">
+        <v>2.333809</v>
+      </c>
+      <c r="N62" s="18">
+        <v>4.4279390000000003</v>
+      </c>
+      <c r="O62" s="18">
+        <v>5.1935979999999997</v>
+      </c>
+      <c r="P62" s="18">
+        <v>6.3916199999999996</v>
+      </c>
+      <c r="Q62" s="18">
+        <v>7.7538210000000003</v>
+      </c>
+      <c r="R62" s="18">
+        <v>8.6599590000000006</v>
+      </c>
+      <c r="S62" s="18">
+        <v>9.586608</v>
+      </c>
+      <c r="T62" s="18">
+        <v>10.808149999999999</v>
+      </c>
+      <c r="U62" s="18">
+        <v>12.165281999999999</v>
+      </c>
+      <c r="V62" s="18">
+        <v>13.189172000000001</v>
+      </c>
+      <c r="W62" s="18">
+        <v>15.356909999999999</v>
+      </c>
+      <c r="X62" s="18">
+        <v>19.984625000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="16">
+        <v>4.8159999999999994E-2</v>
+      </c>
+      <c r="C63" s="16">
+        <v>0.13124</v>
+      </c>
+      <c r="D63" s="16">
+        <v>0.26558999999999999</v>
+      </c>
+      <c r="E63" s="16">
+        <v>0.38774999999999998</v>
+      </c>
+      <c r="F63" s="16">
+        <v>0.59484999999999999</v>
+      </c>
+      <c r="G63" s="16">
+        <v>0.96257000000000004</v>
+      </c>
+      <c r="H63" s="16">
+        <v>2.1825799999999997</v>
+      </c>
+      <c r="I63" s="16">
+        <v>4.0701100000000006</v>
+      </c>
+      <c r="J63" s="16">
+        <v>5.69421</v>
+      </c>
+      <c r="K63" s="16">
+        <v>7.9115699999999993</v>
+      </c>
+      <c r="L63" s="16">
+        <v>9.9449900000000007</v>
+      </c>
+      <c r="M63" s="16">
+        <v>12.371619000000001</v>
+      </c>
+      <c r="N63" s="16">
+        <v>15.1784</v>
+      </c>
+      <c r="O63" s="16">
+        <v>16.137004999999998</v>
+      </c>
+      <c r="P63" s="16">
+        <v>17.323777</v>
+      </c>
+      <c r="Q63" s="16">
+        <v>21.420601999999999</v>
+      </c>
+      <c r="R63" s="16">
+        <v>21.380984999999999</v>
+      </c>
+      <c r="S63" s="16">
+        <v>24.609437000000003</v>
+      </c>
+      <c r="T63" s="16">
+        <v>28.598595</v>
+      </c>
+      <c r="U63" s="16">
+        <v>34.721682999999999</v>
+      </c>
+      <c r="V63" s="16">
+        <v>40.045404000000005</v>
+      </c>
+      <c r="W63" s="16">
+        <v>37.119413000000002</v>
+      </c>
+      <c r="X63" s="16">
+        <v>38.004227</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A67" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A68" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C68" s="10">
+        <v>2001</v>
+      </c>
+      <c r="D68" s="10">
+        <v>2002</v>
+      </c>
+      <c r="E68" s="10">
+        <v>2003</v>
+      </c>
+      <c r="F68" s="10">
+        <v>2004</v>
+      </c>
+      <c r="G68" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H68" s="10">
+        <v>2006</v>
+      </c>
+      <c r="I68" s="10">
+        <v>2007</v>
+      </c>
+      <c r="J68" s="10">
+        <v>2008</v>
+      </c>
+      <c r="K68" s="10">
+        <v>2009</v>
+      </c>
+      <c r="L68" s="10">
+        <v>2010</v>
+      </c>
+      <c r="M68" s="10">
+        <v>2011</v>
+      </c>
+      <c r="N68" s="10">
+        <v>2012</v>
+      </c>
+      <c r="O68" s="10">
+        <v>2013</v>
+      </c>
+      <c r="P68" s="10">
+        <v>2014</v>
+      </c>
+      <c r="Q68" s="10">
+        <v>2015</v>
+      </c>
+      <c r="R68" s="10">
+        <v>2016</v>
+      </c>
+      <c r="S68" s="10">
+        <v>2017</v>
+      </c>
+      <c r="T68" s="10">
+        <v>2018</v>
+      </c>
+      <c r="U68" s="10">
+        <v>2019</v>
+      </c>
+      <c r="V68" s="10">
+        <v>2020</v>
+      </c>
+      <c r="W68" s="10">
+        <v>2021</v>
+      </c>
+      <c r="X68" s="10">
+        <v>2022</v>
+      </c>
+      <c r="Y68" s="10">
+        <v>2023</v>
+      </c>
+      <c r="Z68" s="10">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A69" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="15">
+        <v>0.432</v>
+      </c>
+      <c r="C69" s="15">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="D69" s="15">
+        <v>0.52849999999999997</v>
+      </c>
+      <c r="E69" s="15">
+        <v>0.55149999999999999</v>
+      </c>
+      <c r="F69" s="15">
+        <v>0.60550000000000004</v>
+      </c>
+      <c r="G69" s="15">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H69" s="15">
+        <v>0.66749999999999998</v>
+      </c>
+      <c r="I69" s="15">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="J69" s="15">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="K69" s="15">
+        <v>0.8175</v>
+      </c>
+      <c r="L69" s="15">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="M69" s="15">
+        <v>1.1749360000000002</v>
+      </c>
+      <c r="N69" s="15">
+        <v>1.281048</v>
+      </c>
+      <c r="O69" s="15">
+        <v>1.4079560000000002</v>
+      </c>
+      <c r="P69" s="15">
+        <v>1.4632609999999999</v>
+      </c>
+      <c r="Q69" s="15">
+        <v>1.531277</v>
+      </c>
+      <c r="R69" s="15">
+        <v>1.6606730000000001</v>
+      </c>
+      <c r="S69" s="15">
+        <v>1.7124410000000001</v>
+      </c>
+      <c r="T69" s="15">
+        <v>1.9245109999999999</v>
+      </c>
+      <c r="U69" s="15">
+        <v>2.0081630000000001</v>
+      </c>
+      <c r="V69" s="15">
+        <v>1.931778</v>
+      </c>
+      <c r="W69" s="15">
+        <v>2.0463560000000003</v>
+      </c>
+      <c r="X69" s="15">
+        <v>2.0585360000000001</v>
+      </c>
+      <c r="Y69" s="15">
+        <v>2.0904589999999996</v>
+      </c>
+      <c r="Z69" s="15">
+        <v>3.3514589999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A70" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17">
+        <v>1.49E-2</v>
+      </c>
+      <c r="N70" s="17">
+        <v>1.35E-2</v>
+      </c>
+      <c r="O70" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P70" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q70" s="17">
+        <v>1.4749999999999999E-2</v>
+      </c>
+      <c r="R70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="S70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="T70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="U70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="V70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="W70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="X70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="Y70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+      <c r="Z70" s="17">
+        <v>1.6149999999999998E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A71" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="15">
+        <v>25.154</v>
+      </c>
+      <c r="C71" s="15">
+        <v>25.178999999999998</v>
+      </c>
+      <c r="D71" s="15">
+        <v>25.277999999999999</v>
+      </c>
+      <c r="E71" s="15">
+        <v>25.23</v>
+      </c>
+      <c r="F71" s="15">
+        <v>25.117000000000001</v>
+      </c>
+      <c r="G71" s="15">
+        <v>25.13</v>
+      </c>
+      <c r="H71" s="15">
+        <v>25.141999999999999</v>
+      </c>
+      <c r="I71" s="15">
+        <v>25.155000000000001</v>
+      </c>
+      <c r="J71" s="15">
+        <v>25.12</v>
+      </c>
+      <c r="K71" s="15">
+        <v>25.207999999999998</v>
+      </c>
+      <c r="L71" s="15">
+        <v>25.425000000000001</v>
+      </c>
+      <c r="M71" s="15">
+        <v>25.641577000000002</v>
+      </c>
+      <c r="N71" s="15">
+        <v>25.655922999999998</v>
+      </c>
+      <c r="O71" s="15">
+        <v>25.645355000000002</v>
+      </c>
+      <c r="P71" s="15">
+        <v>25.526268000000002</v>
+      </c>
+      <c r="Q71" s="15">
+        <v>25.551829000000001</v>
+      </c>
+      <c r="R71" s="15">
+        <v>25.620853000000004</v>
+      </c>
+      <c r="S71" s="15">
+        <v>25.706938000000001</v>
+      </c>
+      <c r="T71" s="15">
+        <v>25.726934</v>
+      </c>
+      <c r="U71" s="15">
+        <v>25.868384000000002</v>
+      </c>
+      <c r="V71" s="15">
+        <v>25.954382000000003</v>
+      </c>
+      <c r="W71" s="15">
+        <v>25.990796000000003</v>
+      </c>
+      <c r="X71" s="15">
+        <v>25.963666</v>
+      </c>
+      <c r="Y71" s="15">
+        <v>26.325191</v>
+      </c>
+      <c r="Z71" s="15">
+        <v>26.846190999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A72" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="17">
+        <v>63.183</v>
+      </c>
+      <c r="C72" s="17">
+        <v>63.183</v>
+      </c>
+      <c r="D72" s="17">
+        <v>63.273000000000003</v>
+      </c>
+      <c r="E72" s="17">
+        <v>63.363</v>
+      </c>
+      <c r="F72" s="17">
+        <v>63.363</v>
+      </c>
+      <c r="G72" s="17">
+        <v>63.26</v>
+      </c>
+      <c r="H72" s="17">
+        <v>63.26</v>
+      </c>
+      <c r="I72" s="17">
+        <v>63.26</v>
+      </c>
+      <c r="J72" s="17">
+        <v>63.26</v>
+      </c>
+      <c r="K72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="L72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="M72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="N72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="O72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="P72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="Q72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="R72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="S72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="T72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="U72" s="17">
+        <v>63.13</v>
+      </c>
+      <c r="V72" s="17">
+        <v>61.4</v>
+      </c>
+      <c r="W72" s="17">
+        <v>61.4</v>
+      </c>
+      <c r="X72" s="17">
+        <v>61.4</v>
+      </c>
+      <c r="Y72" s="17">
+        <v>61.4</v>
+      </c>
+      <c r="Z72" s="17">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A73" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="15">
+        <v>25.491</v>
+      </c>
+      <c r="C73" s="15">
+        <v>26.4</v>
+      </c>
+      <c r="D73" s="15">
+        <v>27.1815</v>
+      </c>
+      <c r="E73" s="15">
+        <v>26.804500000000001</v>
+      </c>
+      <c r="F73" s="15">
+        <v>26.499500000000001</v>
+      </c>
+      <c r="G73" s="15">
+        <v>25.788</v>
+      </c>
+      <c r="H73" s="15">
+        <v>25.0075</v>
+      </c>
+      <c r="I73" s="15">
+        <v>24.806999999999999</v>
+      </c>
+      <c r="J73" s="15">
+        <v>24.705500000000001</v>
+      </c>
+      <c r="K73" s="15">
+        <v>26.291499999999999</v>
+      </c>
+      <c r="L73" s="15">
+        <v>27.483499999999999</v>
+      </c>
+      <c r="M73" s="15">
+        <v>27.429006000000001</v>
+      </c>
+      <c r="N73" s="15">
+        <v>26.576404</v>
+      </c>
+      <c r="O73" s="15">
+        <v>24.455964999999999</v>
+      </c>
+      <c r="P73" s="15">
+        <v>22.754127</v>
+      </c>
+      <c r="Q73" s="15">
+        <v>24.463165</v>
+      </c>
+      <c r="R73" s="15">
+        <v>23.193792000000002</v>
+      </c>
+      <c r="S73" s="15">
+        <v>20.150646000000002</v>
+      </c>
+      <c r="T73" s="15">
+        <v>18.830272999999998</v>
+      </c>
+      <c r="U73" s="15">
+        <v>18.777677000000001</v>
+      </c>
+      <c r="V73" s="15">
+        <v>19.048099000000001</v>
+      </c>
+      <c r="W73" s="15">
+        <v>19.364996999999999</v>
+      </c>
+      <c r="X73" s="15">
+        <v>20.934428</v>
+      </c>
+      <c r="Y73" s="15">
+        <v>19.744399000000001</v>
+      </c>
+      <c r="Z73" s="15">
+        <v>18.819399000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A74" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C74" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D74" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E74" s="17">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F74" s="17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G74" s="17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H74" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I74" s="17">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="J74" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="K74" s="17">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="L74" s="17">
+        <v>1.044</v>
+      </c>
+      <c r="M74" s="17">
+        <v>2.9885770000000003</v>
+      </c>
+      <c r="N74" s="17">
+        <v>4.3007569999999999</v>
+      </c>
+      <c r="O74" s="17">
+        <v>5.1602830000000006</v>
+      </c>
+      <c r="P74" s="17">
+        <v>5.8614049999999995</v>
+      </c>
+      <c r="Q74" s="17">
+        <v>6.8195389999999998</v>
+      </c>
+      <c r="R74" s="17">
+        <v>7.3190770000000001</v>
+      </c>
+      <c r="S74" s="17">
+        <v>8.1004109999999994</v>
+      </c>
+      <c r="T74" s="17">
+        <v>9.0316399999999994</v>
+      </c>
+      <c r="U74" s="17">
+        <v>10.01318</v>
+      </c>
+      <c r="V74" s="17">
+        <v>11.133255999999999</v>
+      </c>
+      <c r="W74" s="17">
+        <v>13.446042</v>
+      </c>
+      <c r="X74" s="17">
+        <v>14.721789000000001</v>
+      </c>
+      <c r="Y74" s="17">
+        <v>17.399135999999999</v>
+      </c>
+      <c r="Z74" s="17">
+        <v>21.528088</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A75" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="15">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C75" s="15">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D75" s="15">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E75" s="15">
+        <v>0.218</v>
+      </c>
+      <c r="F75" s="15">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="G75" s="15">
+        <v>0.69</v>
+      </c>
+      <c r="H75" s="15">
+        <v>1.4119999999999999</v>
+      </c>
+      <c r="I75" s="15">
+        <v>2.2229999999999999</v>
+      </c>
+      <c r="J75" s="15">
+        <v>3.403</v>
+      </c>
+      <c r="K75" s="15">
+        <v>4.5819999999999999</v>
+      </c>
+      <c r="L75" s="15">
+        <v>5.9119999999999999</v>
+      </c>
+      <c r="M75" s="15">
+        <v>6.7580160000000005</v>
+      </c>
+      <c r="N75" s="15">
+        <v>7.6074960000000003</v>
+      </c>
+      <c r="O75" s="15">
+        <v>8.1601309999999998</v>
+      </c>
+      <c r="P75" s="15">
+        <v>9.201394999999998</v>
+      </c>
+      <c r="Q75" s="15">
+        <v>10.298146999999998</v>
+      </c>
+      <c r="R75" s="15">
+        <v>11.566561999999999</v>
+      </c>
+      <c r="S75" s="15">
+        <v>13.499351999999998</v>
+      </c>
+      <c r="T75" s="15">
+        <v>14.900143</v>
+      </c>
+      <c r="U75" s="15">
+        <v>16.426852</v>
+      </c>
+      <c r="V75" s="15">
+        <v>17.535273</v>
+      </c>
+      <c r="W75" s="15">
+        <v>18.551120999999998</v>
+      </c>
+      <c r="X75" s="15">
+        <v>20.835175</v>
+      </c>
+      <c r="Y75" s="15">
+        <v>23.131614000000003</v>
+      </c>
+      <c r="Z75" s="15">
+        <v>24.591614</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A85" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A86" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" s="10">
+        <v>2000</v>
+      </c>
+      <c r="D86" s="10">
+        <v>2001</v>
+      </c>
+      <c r="E86" s="10">
+        <v>2002</v>
+      </c>
+      <c r="F86" s="10">
+        <v>2003</v>
+      </c>
+      <c r="G86" s="10">
+        <v>2004</v>
+      </c>
+      <c r="H86" s="10">
+        <v>2005</v>
+      </c>
+      <c r="I86" s="10">
+        <v>2006</v>
+      </c>
+      <c r="J86" s="10">
+        <v>2007</v>
+      </c>
+      <c r="K86" s="10">
+        <v>2008</v>
+      </c>
+      <c r="L86" s="10">
+        <v>2009</v>
+      </c>
+      <c r="M86" s="10">
+        <v>2010</v>
+      </c>
+      <c r="N86" s="10">
+        <v>2011</v>
+      </c>
+      <c r="O86" s="10">
+        <v>2012</v>
+      </c>
+      <c r="P86" s="10">
+        <v>2013</v>
+      </c>
+      <c r="Q86" s="10">
+        <v>2014</v>
+      </c>
+      <c r="R86" s="10">
+        <v>2015</v>
+      </c>
+      <c r="S86" s="10">
+        <v>2016</v>
+      </c>
+      <c r="T86" s="10">
+        <v>2017</v>
+      </c>
+      <c r="U86" s="10">
+        <v>2018</v>
+      </c>
+      <c r="V86" s="10">
+        <v>2019</v>
+      </c>
+      <c r="W86" s="10">
+        <v>2020</v>
+      </c>
+      <c r="X86" s="10">
+        <v>2021</v>
+      </c>
+      <c r="Y86" s="10">
+        <v>2022</v>
+      </c>
+      <c r="Z86" s="10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A87" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="16">
+        <v>0</v>
+      </c>
+      <c r="D87" s="16">
+        <v>0</v>
+      </c>
+      <c r="E87" s="16">
+        <v>0</v>
+      </c>
+      <c r="F87" s="16">
+        <v>0</v>
+      </c>
+      <c r="G87" s="16">
+        <v>0</v>
+      </c>
+      <c r="H87" s="16">
+        <v>0</v>
+      </c>
+      <c r="I87" s="16">
+        <v>0</v>
+      </c>
+      <c r="J87" s="16">
+        <v>0</v>
+      </c>
+      <c r="K87" s="16">
+        <v>0</v>
+      </c>
+      <c r="L87" s="16">
+        <v>0</v>
+      </c>
+      <c r="M87" s="16">
+        <v>0</v>
+      </c>
+      <c r="N87" s="16">
+        <v>0</v>
+      </c>
+      <c r="O87" s="16">
+        <v>0</v>
+      </c>
+      <c r="P87" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="16">
+        <v>0</v>
+      </c>
+      <c r="R87" s="16">
+        <v>0</v>
+      </c>
+      <c r="S87" s="16">
+        <v>0</v>
+      </c>
+      <c r="T87" s="16">
+        <v>0</v>
+      </c>
+      <c r="U87" s="16">
+        <v>0</v>
+      </c>
+      <c r="V87" s="16">
+        <v>0</v>
+      </c>
+      <c r="W87" s="16">
+        <v>0</v>
+      </c>
+      <c r="X87" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y87" s="16">
+        <v>14.94</v>
+      </c>
+      <c r="Z87" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A88" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" s="18">
+        <v>69.48</v>
+      </c>
+      <c r="D88" s="18">
+        <v>68.39</v>
+      </c>
+      <c r="E88" s="18">
+        <v>77.03</v>
+      </c>
+      <c r="F88" s="18">
+        <v>66.41</v>
+      </c>
+      <c r="G88" s="18">
+        <v>61.91</v>
+      </c>
+      <c r="H88" s="18">
+        <v>60.33</v>
+      </c>
+      <c r="I88" s="18">
+        <v>63.34</v>
+      </c>
+      <c r="J88" s="18">
+        <v>56.81</v>
+      </c>
+      <c r="K88" s="18">
+        <v>47.99</v>
+      </c>
+      <c r="L88" s="18">
+        <v>25.93</v>
+      </c>
+      <c r="M88" s="18">
+        <v>30.71</v>
+      </c>
+      <c r="N88" s="18">
+        <v>56.41</v>
+      </c>
+      <c r="O88" s="18">
+        <v>44.52</v>
+      </c>
+      <c r="P88" s="18">
+        <v>48.46</v>
+      </c>
+      <c r="Q88" s="18">
+        <v>67.19</v>
+      </c>
+      <c r="R88" s="18">
+        <v>64.06</v>
+      </c>
+      <c r="S88" s="18">
+        <v>41.5</v>
+      </c>
+      <c r="T88" s="18">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="U88" s="18">
+        <v>62.97</v>
+      </c>
+      <c r="V88" s="18">
+        <v>57.67</v>
+      </c>
+      <c r="W88" s="18">
+        <v>45.04</v>
+      </c>
+      <c r="X88" s="18">
+        <v>44.89</v>
+      </c>
+      <c r="Y88" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z88" s="18">
+        <v>50.34</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Y1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>